<commit_message>
Work for 2023-0219, morning of 2023-0220: Adjusting the variables.xlsx file, setting up the files and symlinks for the featureCounts work
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D7A61-2E16-0C49-93AC-6E51F99336DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B96E8AF-54E6-834E-9537-F11713FC86D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="master" sheetId="1" r:id="rId1"/>
+    <sheet name="aligned_UTK_primary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="379">
   <si>
     <t>5781_G1_IN</t>
   </si>
@@ -639,13 +640,547 @@
   </si>
   <si>
     <t>WT_Q_N_rep4</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_N_rep1</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep1</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_N_rep2</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep2</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_SS_rep1</t>
+  </si>
+  <si>
+    <t>t4-n_DSp48_day4_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_DSm2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>t4-n_DSm2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_DSp2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>t4-n_DSp2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_DSp24_day3_SS_rep1</t>
+  </si>
+  <si>
+    <t>t4-n_DSp24_day3_SS_rep1</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_SS_rep2</t>
+  </si>
+  <si>
+    <t>t4-n_DSp48_day4_SS_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_DSm2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>t4-n_DSm2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_DSp2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>t4-n_DSp2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_DSp24_day3_SS_rep2</t>
+  </si>
+  <si>
+    <t>t4-n_DSp24_day3_SS_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_rep2</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep2</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep2</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_N_rep1</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_SS_rep1</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_N_rep2</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_SS_rep2</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep1</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep1</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_SS_rep1</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_N_rep1</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_SS_rep2</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_N_rep2</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_SS_rep1</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_N_rep1</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_SS_rep2</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_N_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_SS_rep1</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_N_rep1</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_SS_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_N_rep2</t>
+  </si>
+  <si>
+    <t>5781_G1_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5781_G1_IP_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5781_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5781_Q_IP_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5782_G1_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5782_G1_IP_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5782_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>5782_Q_IP_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM10_DSp48_5781_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM11_DSp48_7080_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM1_DSm2_5781_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM2_DSm2_7080_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM3_DSm2_7079_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM4_DSp2_5781_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM5_DSp2_7080_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM6_DSp2_7079_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM7_DSp24_5781_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM8_DSp24_7080_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>BM9_DSp24_7079_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp10_DSp48_5782_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp11_DSp48_7081_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp12_DSp48_7078_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp1_DSm2_5782_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp2_DSm2_7081_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp3_DSm2_7078_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp4_DSp2_5782_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp5_DSp2_7081_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp6_DSp2_7078_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp7_DSp24_5782_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp8_DSp24_7081_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>Bp9_DSp24_7078_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT10_7718_pIAA_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT10_7718_pIAA_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT2_6125_pIAA_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT2_6125_pIAA_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT4_6126_pIAA_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT4_6126_pIAA_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT6_7714_pIAA_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT6_7714_pIAA_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT8_7716_pIAA_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CT8_7716_pIAA_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CU11_5782_Q_Nascent_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CU12_5782_Q_SteadyState_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW10_7747_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW10_7747_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW12_7748_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW12_7748_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW2_5781_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW2_5781_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW4_5782_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW4_5782_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW6_7078_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW6_7078_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW8_7079_8day_Q_IN_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>CW8_7079_8day_Q_PD_UTK.primary.bam</t>
+  </si>
+  <si>
+    <t>bams</t>
+  </si>
+  <si>
+    <t>sample_rename</t>
+  </si>
+  <si>
+    <t>bams_rename</t>
+  </si>
+  <si>
+    <t>suffix</t>
+  </si>
+  <si>
+    <t>.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_G1_day1_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp48_day4_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSm2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSm2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp24_day3_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp24_day3_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp48_day4_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSm2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSm2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_DSp24_day3_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>t4-n_DSp24_day3_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>o-d_Q_day7_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r1-n_Q_day8_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day8_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_SS_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_N_rep1.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_SS_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_Q_day8_N_rep2.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>rep-5</t>
+  </si>
+  <si>
+    <t>rep5</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>WT_Q_SS_rep5</t>
+  </si>
+  <si>
+    <t>WT_Q_N_rep5</t>
+  </si>
+  <si>
+    <t>name_updated</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep2_CU</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep2_CU</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep3</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep3</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_N_rep3.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>n3-d_Q_day7_SS_rep3.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_N_rep2_CU.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>WT_Q_day7_SS_rep2_CU.UTK_prim.bam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -691,13 +1226,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
@@ -738,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -749,21 +1277,27 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1078,43 +1612,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D52A0-EFB8-324D-84A5-D98AF0E44661}">
-  <dimension ref="A1:AB56"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.5" customWidth="1"/>
+    <col min="29" max="29" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1142,16 +1677,16 @@
       <c r="I1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="10" t="s">
         <v>187</v>
       </c>
       <c r="N1" s="6" t="s">
@@ -1196,15 +1731,18 @@
       <c r="AA1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AB1" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C2" s="2">
@@ -1214,7 +1752,7 @@
         <v>56</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f>D2</f>
+        <f t="shared" ref="E2:E32" si="0">D2</f>
         <v>wild-type</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1229,7 +1767,7 @@
       <c r="I2" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1238,7 +1776,7 @@
       <c r="L2" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N2" s="6" t="s">
@@ -1284,15 +1822,18 @@
         <f>_xlfn.CONCAT(F2, "_", N2, "_", R2, "_", W2, "_", I2)</f>
         <v>WT_G1_day1_SS_rep1</v>
       </c>
-      <c r="AB2" s="19" t="s">
+      <c r="AB2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC2" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="2">
@@ -1302,7 +1843,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f>D3</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1317,7 +1858,7 @@
       <c r="I3" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -1326,7 +1867,7 @@
       <c r="L3" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N3" s="6" t="s">
@@ -1369,18 +1910,21 @@
         <v>131</v>
       </c>
       <c r="AA3" s="2" t="str">
-        <f t="shared" ref="AA3:AA56" si="0">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", W3, "_", I3)</f>
+        <f t="shared" ref="AA3:AB56" si="1">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", W3, "_", I3)</f>
         <v>WT_G1_day1_N_rep1</v>
       </c>
-      <c r="AB3" s="19" t="s">
+      <c r="AB3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC3" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C4" s="2">
@@ -1390,7 +1934,7 @@
         <v>56</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f>D4</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1405,7 +1949,7 @@
       <c r="I4" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1414,7 +1958,7 @@
       <c r="L4" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N4" s="6" t="s">
@@ -1457,18 +2001,21 @@
         <v>131</v>
       </c>
       <c r="AA4" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_SS_rep1</v>
       </c>
-      <c r="AB4" s="17" t="s">
+      <c r="AB4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC4" s="10" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C5" s="2">
@@ -1478,7 +2025,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1493,7 +2040,7 @@
       <c r="I5" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1502,7 +2049,7 @@
       <c r="L5" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N5" s="6" t="s">
@@ -1545,18 +2092,21 @@
         <v>131</v>
       </c>
       <c r="AA5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_N_rep1</v>
       </c>
-      <c r="AB5" s="17" t="s">
+      <c r="AB5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC5" s="10" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C6" s="2">
@@ -1566,7 +2116,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="2" t="str">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1581,7 +2131,7 @@
       <c r="I6" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1590,7 +2140,7 @@
       <c r="L6" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N6" s="6" t="s">
@@ -1633,18 +2183,21 @@
         <v>131</v>
       </c>
       <c r="AA6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_G1_day1_SS_rep2</v>
       </c>
-      <c r="AB6" s="19" t="s">
+      <c r="AB6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC6" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C7" s="2">
@@ -1654,7 +2207,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="2" t="str">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1669,7 +2222,7 @@
       <c r="I7" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1678,7 +2231,7 @@
       <c r="L7" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N7" s="6" t="s">
@@ -1721,18 +2274,21 @@
         <v>131</v>
       </c>
       <c r="AA7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_G1_day1_N_rep2</v>
       </c>
-      <c r="AB7" s="19" t="s">
+      <c r="AB7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC7" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C8" s="2">
@@ -1742,7 +2298,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="2" t="str">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1757,7 +2313,7 @@
       <c r="I8" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1766,7 +2322,7 @@
       <c r="L8" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N8" s="6" t="s">
@@ -1809,18 +2365,21 @@
         <v>131</v>
       </c>
       <c r="AA8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_SS_rep2</v>
       </c>
-      <c r="AB8" s="17" t="s">
+      <c r="AB8" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC8" s="10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="2">
@@ -1830,7 +2389,7 @@
         <v>56</v>
       </c>
       <c r="E9" s="2" t="str">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1845,7 +2404,7 @@
       <c r="I9" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1854,7 +2413,7 @@
       <c r="L9" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N9" s="6" t="s">
@@ -1897,14 +2456,17 @@
         <v>131</v>
       </c>
       <c r="AA9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_N_rep2</v>
       </c>
-      <c r="AB9" s="17" t="s">
+      <c r="AB9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AC9" s="10" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1918,7 +2480,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="2" t="str">
-        <f>D10</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -1933,7 +2495,7 @@
       <c r="I10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1942,7 +2504,7 @@
       <c r="L10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -1985,14 +2547,17 @@
         <v>132</v>
       </c>
       <c r="AA10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep1</v>
       </c>
-      <c r="AB10" s="19" t="s">
+      <c r="AB10" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC10" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -2006,7 +2571,7 @@
         <v>103</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>D11</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -2021,7 +2586,7 @@
       <c r="I11" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K11" s="3" t="s">
@@ -2030,7 +2595,7 @@
       <c r="L11" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="3" t="s">
         <v>71</v>
       </c>
       <c r="N11" s="7" t="s">
@@ -2073,14 +2638,17 @@
         <v>132</v>
       </c>
       <c r="AA11" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp48_day4_SS_rep1</v>
       </c>
-      <c r="AB11" s="18" t="s">
+      <c r="AB11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC11" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2094,7 +2662,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="str">
-        <f>D12</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -2109,7 +2677,7 @@
       <c r="I12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -2118,7 +2686,7 @@
       <c r="L12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -2161,14 +2729,17 @@
         <v>132</v>
       </c>
       <c r="AA12" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB12" s="19" t="s">
+      <c r="AB12" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC12" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2182,7 +2753,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>D13</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -2197,7 +2768,7 @@
       <c r="I13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -2206,7 +2777,7 @@
       <c r="L13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="N13" s="7" t="s">
@@ -2249,14 +2820,17 @@
         <v>132</v>
       </c>
       <c r="AA13" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB13" s="18" t="s">
+      <c r="AB13" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC13" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2270,7 +2844,7 @@
         <v>106</v>
       </c>
       <c r="E14" s="2" t="str">
-        <f>D14</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -2285,7 +2859,7 @@
       <c r="I14" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -2294,7 +2868,7 @@
       <c r="L14" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N14" s="6" t="s">
@@ -2337,14 +2911,17 @@
         <v>132</v>
       </c>
       <c r="AA14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB14" s="19" t="s">
+      <c r="AB14" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC14" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2358,7 +2935,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="2" t="str">
-        <f>D15</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -2373,7 +2950,7 @@
       <c r="I15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2382,7 +2959,7 @@
       <c r="L15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="M15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N15" s="6" t="s">
@@ -2425,14 +3002,17 @@
         <v>132</v>
       </c>
       <c r="AA15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB15" s="19" t="s">
+      <c r="AB15" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC15" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -2446,7 +3026,7 @@
         <v>103</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f>D16</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -2461,7 +3041,7 @@
       <c r="I16" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K16" s="3" t="s">
@@ -2470,7 +3050,7 @@
       <c r="L16" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="N16" s="7" t="s">
@@ -2513,14 +3093,17 @@
         <v>132</v>
       </c>
       <c r="AA16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB16" s="18" t="s">
+      <c r="AB16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC16" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2534,7 +3117,7 @@
         <v>106</v>
       </c>
       <c r="E17" s="2" t="str">
-        <f>D17</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -2549,7 +3132,7 @@
       <c r="I17" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -2558,7 +3141,7 @@
       <c r="L17" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="M17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N17" s="6" t="s">
@@ -2601,14 +3184,17 @@
         <v>132</v>
       </c>
       <c r="AA17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB17" s="19" t="s">
+      <c r="AB17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AC17" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2622,7 +3208,7 @@
         <v>56</v>
       </c>
       <c r="E18" s="2" t="str">
-        <f>D18</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -2637,7 +3223,7 @@
       <c r="I18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -2646,7 +3232,7 @@
       <c r="L18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="M18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N18" s="6" t="s">
@@ -2689,14 +3275,17 @@
         <v>132</v>
       </c>
       <c r="AA18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep1</v>
       </c>
-      <c r="AB18" s="19" t="s">
+      <c r="AB18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC18" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +3299,7 @@
         <v>103</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f>D19</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -2725,7 +3314,7 @@
       <c r="I19" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K19" s="3" t="s">
@@ -2734,7 +3323,7 @@
       <c r="L19" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="3" t="s">
         <v>71</v>
       </c>
       <c r="N19" s="7" t="s">
@@ -2777,14 +3366,17 @@
         <v>132</v>
       </c>
       <c r="AA19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp24_day3_SS_rep1</v>
       </c>
-      <c r="AB19" s="18" t="s">
+      <c r="AB19" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC19" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2798,7 +3390,7 @@
         <v>106</v>
       </c>
       <c r="E20" s="2" t="str">
-        <f>D20</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F20" s="6" t="s">
@@ -2813,7 +3405,7 @@
       <c r="I20" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -2822,7 +3414,7 @@
       <c r="L20" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N20" s="6" t="s">
@@ -2865,14 +3457,17 @@
         <v>132</v>
       </c>
       <c r="AA20" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSp24_day3_SS_rep1</v>
       </c>
-      <c r="AB20" s="19" t="s">
+      <c r="AB20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC20" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2886,7 +3481,7 @@
         <v>56</v>
       </c>
       <c r="E21" s="2" t="str">
-        <f>D21</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -2901,7 +3496,7 @@
       <c r="I21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -2910,7 +3505,7 @@
       <c r="L21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="M21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N21" s="6" t="s">
@@ -2953,14 +3548,17 @@
         <v>132</v>
       </c>
       <c r="AA21" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep2</v>
       </c>
-      <c r="AB21" s="19" t="s">
+      <c r="AB21" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC21" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -2974,7 +3572,7 @@
         <v>103</v>
       </c>
       <c r="E22" s="3" t="str">
-        <f>D22</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F22" s="7" t="s">
@@ -2989,7 +3587,7 @@
       <c r="I22" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K22" s="3" t="s">
@@ -2998,7 +3596,7 @@
       <c r="L22" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="3" t="s">
         <v>72</v>
       </c>
       <c r="N22" s="7" t="s">
@@ -3041,14 +3639,17 @@
         <v>132</v>
       </c>
       <c r="AA22" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp48_day4_SS_rep2</v>
       </c>
-      <c r="AB22" s="18" t="s">
+      <c r="AB22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC22" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3062,7 +3663,7 @@
         <v>106</v>
       </c>
       <c r="E23" s="2" t="str">
-        <f>D23</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -3077,7 +3678,7 @@
       <c r="I23" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -3086,7 +3687,7 @@
       <c r="L23" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="M23" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N23" s="6" t="s">
@@ -3129,14 +3730,17 @@
         <v>132</v>
       </c>
       <c r="AA23" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSp48_day4_SS_rep2</v>
       </c>
-      <c r="AB23" s="19" t="s">
+      <c r="AB23" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC23" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3150,7 +3754,7 @@
         <v>56</v>
       </c>
       <c r="E24" s="2" t="str">
-        <f>D24</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -3165,7 +3769,7 @@
       <c r="I24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -3174,7 +3778,7 @@
       <c r="L24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="10" t="s">
+      <c r="M24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N24" s="6" t="s">
@@ -3217,14 +3821,17 @@
         <v>132</v>
       </c>
       <c r="AA24" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB24" s="19" t="s">
+      <c r="AB24" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC24" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -3238,7 +3845,7 @@
         <v>103</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>D25</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F25" s="7" t="s">
@@ -3253,7 +3860,7 @@
       <c r="I25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -3262,7 +3869,7 @@
       <c r="L25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M25" s="11" t="s">
+      <c r="M25" s="3" t="s">
         <v>72</v>
       </c>
       <c r="N25" s="7" t="s">
@@ -3305,14 +3912,17 @@
         <v>132</v>
       </c>
       <c r="AA25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB25" s="18" t="s">
+      <c r="AB25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC25" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -3326,7 +3936,7 @@
         <v>106</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f>D26</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -3341,7 +3951,7 @@
       <c r="I26" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -3350,7 +3960,7 @@
       <c r="L26" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="M26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N26" s="6" t="s">
@@ -3393,14 +4003,17 @@
         <v>132</v>
       </c>
       <c r="AA26" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB26" s="19" t="s">
+      <c r="AB26" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC26" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -3414,7 +4027,7 @@
         <v>56</v>
       </c>
       <c r="E27" s="2" t="str">
-        <f>D27</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F27" s="6" t="s">
@@ -3429,7 +4042,7 @@
       <c r="I27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -3438,7 +4051,7 @@
       <c r="L27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="M27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N27" s="6" t="s">
@@ -3481,14 +4094,17 @@
         <v>132</v>
       </c>
       <c r="AA27" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB27" s="19" t="s">
+      <c r="AB27" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC27" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -3502,7 +4118,7 @@
         <v>103</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>D28</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F28" s="7" t="s">
@@ -3517,7 +4133,7 @@
       <c r="I28" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K28" s="3" t="s">
@@ -3526,7 +4142,7 @@
       <c r="L28" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M28" s="11" t="s">
+      <c r="M28" s="3" t="s">
         <v>72</v>
       </c>
       <c r="N28" s="7" t="s">
@@ -3569,14 +4185,17 @@
         <v>132</v>
       </c>
       <c r="AA28" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB28" s="18" t="s">
+      <c r="AB28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC28" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -3590,7 +4209,7 @@
         <v>106</v>
       </c>
       <c r="E29" s="2" t="str">
-        <f>D29</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -3605,7 +4224,7 @@
       <c r="I29" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -3614,7 +4233,7 @@
       <c r="L29" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M29" s="10" t="s">
+      <c r="M29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N29" s="6" t="s">
@@ -3657,14 +4276,17 @@
         <v>132</v>
       </c>
       <c r="AA29" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB29" s="19" t="s">
+      <c r="AB29" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC29" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -3678,7 +4300,7 @@
         <v>56</v>
       </c>
       <c r="E30" s="2" t="str">
-        <f>D30</f>
+        <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -3693,7 +4315,7 @@
       <c r="I30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -3702,7 +4324,7 @@
       <c r="L30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M30" s="10" t="s">
+      <c r="M30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N30" s="6" t="s">
@@ -3745,14 +4367,17 @@
         <v>132</v>
       </c>
       <c r="AA30" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB30" s="19" t="s">
+      <c r="AB30" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC30" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -3766,7 +4391,7 @@
         <v>103</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>D31</f>
+        <f t="shared" si="0"/>
         <v>trf4-null</v>
       </c>
       <c r="F31" s="7" t="s">
@@ -3781,7 +4406,7 @@
       <c r="I31" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K31" s="3" t="s">
@@ -3790,7 +4415,7 @@
       <c r="L31" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="3" t="s">
         <v>72</v>
       </c>
       <c r="N31" s="7" t="s">
@@ -3833,14 +4458,17 @@
         <v>132</v>
       </c>
       <c r="AA31" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>t4-n_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB31" s="18" t="s">
+      <c r="AB31" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC31" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3854,7 +4482,7 @@
         <v>106</v>
       </c>
       <c r="E32" s="2" t="str">
-        <f>D32</f>
+        <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F32" s="6" t="s">
@@ -3869,7 +4497,7 @@
       <c r="I32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -3878,7 +4506,7 @@
       <c r="L32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M32" s="10" t="s">
+      <c r="M32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N32" s="6" t="s">
@@ -3921,14 +4549,17 @@
         <v>132</v>
       </c>
       <c r="AA32" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB32" s="19" t="s">
+      <c r="AB32" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC32" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -3956,7 +4587,7 @@
       <c r="I33" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="4" t="s">
         <v>72</v>
       </c>
       <c r="K33" s="4" t="s">
@@ -3965,7 +4596,7 @@
       <c r="L33" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="M33" s="12" t="s">
+      <c r="M33" s="4" t="s">
         <v>72</v>
       </c>
       <c r="N33" s="6" t="s">
@@ -4008,14 +4639,17 @@
         <v>131</v>
       </c>
       <c r="AA33" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_N_rep2</v>
       </c>
-      <c r="AB33" s="19" t="s">
+      <c r="AB33" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC33" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -4043,7 +4677,7 @@
       <c r="I34" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="4" t="s">
         <v>72</v>
       </c>
       <c r="K34" s="4" t="s">
@@ -4052,7 +4686,7 @@
       <c r="L34" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="M34" s="12" t="s">
+      <c r="M34" s="4" t="s">
         <v>72</v>
       </c>
       <c r="N34" s="6" t="s">
@@ -4095,14 +4729,17 @@
         <v>131</v>
       </c>
       <c r="AA34" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_SS_rep2</v>
       </c>
-      <c r="AB34" s="19" t="s">
+      <c r="AB34" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC34" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -4131,7 +4768,7 @@
       <c r="I35" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K35" s="2" t="s">
@@ -4140,7 +4777,7 @@
       <c r="L35" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="M35" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N35" s="6" t="s">
@@ -4183,14 +4820,17 @@
         <v>131</v>
       </c>
       <c r="AA35" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_N_rep1</v>
       </c>
-      <c r="AB35" s="19" t="s">
+      <c r="AB35" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC35" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -4219,7 +4859,7 @@
       <c r="I36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K36" s="2" t="s">
@@ -4228,7 +4868,7 @@
       <c r="L36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M36" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N36" s="6" t="s">
@@ -4271,14 +4911,17 @@
         <v>131</v>
       </c>
       <c r="AA36" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_SS_rep1</v>
       </c>
-      <c r="AB36" s="19" t="s">
+      <c r="AB36" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC36" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -4307,7 +4950,7 @@
       <c r="I37" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -4316,7 +4959,7 @@
       <c r="L37" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M37" s="10" t="s">
+      <c r="M37" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N37" s="6" t="s">
@@ -4359,14 +5002,17 @@
         <v>131</v>
       </c>
       <c r="AA37" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_N_rep2</v>
       </c>
-      <c r="AB37" s="19" t="s">
+      <c r="AB37" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC37" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -4395,7 +5041,7 @@
       <c r="I38" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K38" s="2" t="s">
@@ -4404,7 +5050,7 @@
       <c r="L38" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M38" s="10" t="s">
+      <c r="M38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N38" s="6" t="s">
@@ -4447,14 +5093,17 @@
         <v>131</v>
       </c>
       <c r="AA38" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_SS_rep2</v>
       </c>
-      <c r="AB38" s="19" t="s">
+      <c r="AB38" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC38" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -4482,7 +5131,7 @@
       <c r="I39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J39" s="12" t="s">
+      <c r="J39" s="4" t="s">
         <v>71</v>
       </c>
       <c r="K39" s="4" t="s">
@@ -4491,7 +5140,7 @@
       <c r="L39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="M39" s="12" t="s">
+      <c r="M39" s="4" t="s">
         <v>71</v>
       </c>
       <c r="N39" s="6" t="s">
@@ -4534,14 +5183,17 @@
         <v>131</v>
       </c>
       <c r="AA39" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_N_rep1</v>
       </c>
-      <c r="AB39" s="19" t="s">
+      <c r="AB39" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC39" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4569,7 +5221,7 @@
       <c r="I40" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J40" s="12" t="s">
+      <c r="J40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="K40" s="4" t="s">
@@ -4578,7 +5230,7 @@
       <c r="L40" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="M40" s="12" t="s">
+      <c r="M40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="N40" s="6" t="s">
@@ -4621,14 +5273,17 @@
         <v>131</v>
       </c>
       <c r="AA40" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_SS_rep1</v>
       </c>
-      <c r="AB40" s="19" t="s">
+      <c r="AB40" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC40" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -4656,7 +5311,7 @@
       <c r="I41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="J41" s="4" t="s">
         <v>73</v>
       </c>
       <c r="K41" s="4" t="s">
@@ -4665,7 +5320,7 @@
       <c r="L41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="M41" s="12" t="s">
+      <c r="M41" s="4" t="s">
         <v>73</v>
       </c>
       <c r="N41" s="6" t="s">
@@ -4708,14 +5363,17 @@
         <v>131</v>
       </c>
       <c r="AA41" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_N_rep1</v>
       </c>
-      <c r="AB41" s="19" t="s">
+      <c r="AB41" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="AC41" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -4743,7 +5401,7 @@
       <c r="I42" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="4" t="s">
         <v>73</v>
       </c>
       <c r="K42" s="4" t="s">
@@ -4752,7 +5410,7 @@
       <c r="L42" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="M42" s="12" t="s">
+      <c r="M42" s="4" t="s">
         <v>73</v>
       </c>
       <c r="N42" s="6" t="s">
@@ -4795,14 +5453,17 @@
         <v>131</v>
       </c>
       <c r="AA42" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_SS_rep1</v>
       </c>
-      <c r="AB42" s="19" t="s">
+      <c r="AB42" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="AC42" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -4816,7 +5477,7 @@
         <v>56</v>
       </c>
       <c r="E43" s="2" t="str">
-        <f>D43</f>
+        <f t="shared" ref="E43:E56" si="2">D43</f>
         <v>wild-type</v>
       </c>
       <c r="F43" s="6" t="s">
@@ -4831,17 +5492,17 @@
       <c r="I43" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="J43" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>138</v>
+      <c r="K43" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="M43" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>59</v>
@@ -4883,14 +5544,17 @@
         <v>131</v>
       </c>
       <c r="AA43" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_N_rep2</v>
       </c>
-      <c r="AB43" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB43" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="AC43" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -4904,7 +5568,7 @@
         <v>56</v>
       </c>
       <c r="E44" s="2" t="str">
-        <f>D44</f>
+        <f t="shared" si="2"/>
         <v>wild-type</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -4919,17 +5583,17 @@
       <c r="I44" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="J44" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L44" s="6" t="s">
-        <v>138</v>
+      <c r="K44" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L44" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N44" s="6" t="s">
         <v>59</v>
@@ -4971,14 +5635,17 @@
         <v>131</v>
       </c>
       <c r="AA44" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_SS_rep2</v>
       </c>
-      <c r="AB44" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB44" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="AC44" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -4992,7 +5659,7 @@
         <v>117</v>
       </c>
       <c r="E45" s="2" t="str">
-        <f>D45</f>
+        <f t="shared" si="2"/>
         <v>rtr1-null</v>
       </c>
       <c r="F45" s="6" t="s">
@@ -5007,7 +5674,7 @@
       <c r="I45" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K45" s="2" t="s">
@@ -5016,7 +5683,7 @@
       <c r="L45" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M45" s="10" t="s">
+      <c r="M45" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N45" s="6" t="s">
@@ -5059,14 +5726,17 @@
         <v>131</v>
       </c>
       <c r="AA45" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_SS_rep1</v>
       </c>
-      <c r="AB45" s="19" t="s">
+      <c r="AB45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC45" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -5080,7 +5750,7 @@
         <v>117</v>
       </c>
       <c r="E46" s="2" t="str">
-        <f>D46</f>
+        <f t="shared" si="2"/>
         <v>rtr1-null</v>
       </c>
       <c r="F46" s="6" t="s">
@@ -5095,7 +5765,7 @@
       <c r="I46" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J46" s="10" t="s">
+      <c r="J46" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K46" s="2" t="s">
@@ -5104,7 +5774,7 @@
       <c r="L46" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M46" s="10" t="s">
+      <c r="M46" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N46" s="6" t="s">
@@ -5147,14 +5817,17 @@
         <v>131</v>
       </c>
       <c r="AA46" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_N_rep1</v>
       </c>
-      <c r="AB46" s="19" t="s">
+      <c r="AB46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC46" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -5168,7 +5841,7 @@
         <v>117</v>
       </c>
       <c r="E47" s="2" t="str">
-        <f>D47</f>
+        <f t="shared" si="2"/>
         <v>rtr1-null</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -5183,7 +5856,7 @@
       <c r="I47" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K47" s="2" t="s">
@@ -5192,7 +5865,7 @@
       <c r="L47" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M47" s="10" t="s">
+      <c r="M47" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N47" s="6" t="s">
@@ -5235,14 +5908,17 @@
         <v>131</v>
       </c>
       <c r="AA47" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_SS_rep2</v>
       </c>
-      <c r="AB47" s="19" t="s">
+      <c r="AB47" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC47" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -5256,7 +5932,7 @@
         <v>117</v>
       </c>
       <c r="E48" s="2" t="str">
-        <f>D48</f>
+        <f t="shared" si="2"/>
         <v>rtr1-null</v>
       </c>
       <c r="F48" s="6" t="s">
@@ -5271,7 +5947,7 @@
       <c r="I48" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J48" s="10" t="s">
+      <c r="J48" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K48" s="2" t="s">
@@ -5280,7 +5956,7 @@
       <c r="L48" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M48" s="10" t="s">
+      <c r="M48" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N48" s="6" t="s">
@@ -5323,14 +5999,17 @@
         <v>131</v>
       </c>
       <c r="AA48" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_N_rep2</v>
       </c>
-      <c r="AB48" s="19" t="s">
+      <c r="AB48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="AC48" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -5344,7 +6023,7 @@
         <v>56</v>
       </c>
       <c r="E49" s="2" t="str">
-        <f>D49</f>
+        <f t="shared" si="2"/>
         <v>wild-type</v>
       </c>
       <c r="F49" s="6" t="s">
@@ -5359,17 +6038,17 @@
       <c r="I49" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J49" s="10" t="s">
+      <c r="J49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K49" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="L49" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="M49" s="16" t="s">
-        <v>73</v>
+      <c r="K49" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="M49" s="10" t="s">
+        <v>191</v>
       </c>
       <c r="N49" s="6" t="s">
         <v>59</v>
@@ -5411,14 +6090,17 @@
         <v>131</v>
       </c>
       <c r="AA49" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_SS_rep1</v>
       </c>
-      <c r="AB49" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB49" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC49" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -5432,7 +6114,7 @@
         <v>56</v>
       </c>
       <c r="E50" s="2" t="str">
-        <f>D50</f>
+        <f t="shared" si="2"/>
         <v>wild-type</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -5447,17 +6129,17 @@
       <c r="I50" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K50" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="L50" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="M50" s="16" t="s">
-        <v>73</v>
+      <c r="K50" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="M50" s="10" t="s">
+        <v>191</v>
       </c>
       <c r="N50" s="6" t="s">
         <v>59</v>
@@ -5499,14 +6181,17 @@
         <v>131</v>
       </c>
       <c r="AA50" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_N_rep1</v>
       </c>
-      <c r="AB50" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB50" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -5520,7 +6205,7 @@
         <v>56</v>
       </c>
       <c r="E51" s="2" t="str">
-        <f>D51</f>
+        <f t="shared" si="2"/>
         <v>wild-type</v>
       </c>
       <c r="F51" s="6" t="s">
@@ -5535,17 +6220,17 @@
       <c r="I51" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="J51" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K51" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="M51" s="16" t="s">
-        <v>191</v>
+      <c r="K51" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="L51" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="M51" s="10" t="s">
+        <v>367</v>
       </c>
       <c r="N51" s="6" t="s">
         <v>59</v>
@@ -5587,14 +6272,17 @@
         <v>131</v>
       </c>
       <c r="AA51" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_SS_rep2</v>
       </c>
-      <c r="AB51" s="17" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB51" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC51" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
@@ -5608,7 +6296,7 @@
         <v>56</v>
       </c>
       <c r="E52" s="2" t="str">
-        <f>D52</f>
+        <f t="shared" si="2"/>
         <v>wild-type</v>
       </c>
       <c r="F52" s="6" t="s">
@@ -5623,17 +6311,17 @@
       <c r="I52" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="J52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K52" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="L52" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="M52" s="16" t="s">
-        <v>191</v>
+      <c r="K52" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="M52" s="10" t="s">
+        <v>367</v>
       </c>
       <c r="N52" s="6" t="s">
         <v>59</v>
@@ -5675,14 +6363,17 @@
         <v>131</v>
       </c>
       <c r="AA52" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_N_rep2</v>
       </c>
-      <c r="AB52" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB52" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC52" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -5696,7 +6387,7 @@
         <v>106</v>
       </c>
       <c r="E53" s="2" t="str">
-        <f>D53</f>
+        <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F53" s="6" t="s">
@@ -5711,7 +6402,7 @@
       <c r="I53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="J53" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K53" s="2" t="s">
@@ -5720,7 +6411,7 @@
       <c r="L53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M53" s="10" t="s">
+      <c r="M53" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N53" s="6" t="s">
@@ -5763,14 +6454,17 @@
         <v>131</v>
       </c>
       <c r="AA53" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep1</v>
       </c>
-      <c r="AB53" s="19" t="s">
+      <c r="AB53" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC53" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -5784,7 +6478,7 @@
         <v>106</v>
       </c>
       <c r="E54" s="2" t="str">
-        <f>D54</f>
+        <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F54" s="6" t="s">
@@ -5799,7 +6493,7 @@
       <c r="I54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K54" s="2" t="s">
@@ -5808,7 +6502,7 @@
       <c r="L54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M54" s="10" t="s">
+      <c r="M54" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N54" s="6" t="s">
@@ -5851,14 +6545,17 @@
         <v>131</v>
       </c>
       <c r="AA54" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep1</v>
       </c>
-      <c r="AB54" s="19" t="s">
+      <c r="AB54" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC54" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -5872,7 +6569,7 @@
         <v>106</v>
       </c>
       <c r="E55" s="2" t="str">
-        <f>D55</f>
+        <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F55" s="6" t="s">
@@ -5887,7 +6584,7 @@
       <c r="I55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="J55" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -5896,7 +6593,7 @@
       <c r="L55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M55" s="10" t="s">
+      <c r="M55" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N55" s="6" t="s">
@@ -5939,14 +6636,17 @@
         <v>131</v>
       </c>
       <c r="AA55" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep2</v>
       </c>
-      <c r="AB55" s="19" t="s">
+      <c r="AB55" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC55" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -5960,7 +6660,7 @@
         <v>106</v>
       </c>
       <c r="E56" s="2" t="str">
-        <f>D56</f>
+        <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F56" s="6" t="s">
@@ -5975,7 +6675,7 @@
       <c r="I56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="2" t="s">
         <v>72</v>
       </c>
       <c r="K56" s="2" t="s">
@@ -5984,7 +6684,7 @@
       <c r="L56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M56" s="10" t="s">
+      <c r="M56" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N56" s="6" t="s">
@@ -6027,14 +6727,1386 @@
         <v>131</v>
       </c>
       <c r="AA56" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep2</v>
       </c>
-      <c r="AB56" s="19" t="s">
+      <c r="AB56" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC56" s="13" t="s">
         <v>148</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6671224-CAF5-E647-BCC4-AFC80FBAC049}">
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>_xlfn.CONCAT(C2, E2)</f>
+        <v>WT_G1_day1_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f t="shared" ref="D3:D56" si="0">_xlfn.CONCAT(C3, E3)</f>
+        <v>WT_G1_day1_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_G1_day1_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_G1_day1_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp48_day4_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp48_day4_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSm2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp24_day3_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp24_day3_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSp24_day3_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp48_day4_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp48_day4_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSp48_day4_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSm2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_DSp24_day3_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>t4-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>o-d_Q_day7_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>o-d_Q_day7_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>o-d_Q_day7_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>o-d_Q_day7_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_N_rep3.UTK_prim.bam</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>n3-d_Q_day7_SS_rep3.UTK_prim.bam</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="D43" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_N_rep2_CU.UTK_prim.bam</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D44" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day7_SS_rep2_CU.UTK_prim.bam</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r1-n_Q_day8_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r1-n_Q_day8_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r1-n_Q_day8_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r1-n_Q_day8_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day8_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day8_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day8_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WT_Q_day8_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_Q_day8_SS_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_Q_day8_N_rep1.UTK_prim.bam</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_Q_day8_SS_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>r6-n_Q_day8_N_rep2.UTK_prim.bam</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G56">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work for 2023-0220: Fixing my calls to rnaQUAST and getting initial results; fixing my renamed symlinks to bams and getting the test and real calls to featureCounts working
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B96E8AF-54E6-834E-9537-F11713FC86D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4905C3AC-5DFB-3E4B-B281-D42EF9650B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="51200" yWindow="7700" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="aligned_UTK_primary" sheetId="2" r:id="rId2"/>
+    <sheet name="fix work_count_features.md" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="391">
   <si>
     <t>5781_G1_IN</t>
   </si>
@@ -1174,13 +1175,67 @@
   </si>
   <si>
     <t>WT_Q_day7_SS_rep2_CU.UTK_prim.bam</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_SS_rep1</t>
+  </si>
+  <si>
+    <t>incorrect</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>intermediate</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_x-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_x-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_x-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSm2_day2_SS_y-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSp2_day2_SS_y-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSp24_day3_SS_y-dekho</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_SS_y-dekho</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>#TODO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> replace x-dekho with rep2; replace y-dekho with rep1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1239,6 +1294,13 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1266,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1281,7 +1343,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D52A0-EFB8-324D-84A5-D98AF0E44661}">
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="111" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1910,7 +1976,7 @@
         <v>131</v>
       </c>
       <c r="AA3" s="2" t="str">
-        <f t="shared" ref="AA3:AB56" si="1">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", W3, "_", I3)</f>
+        <f t="shared" ref="AA3:AA56" si="1">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", W3, "_", I3)</f>
         <v>WT_G1_day1_N_rep1</v>
       </c>
       <c r="AB3" s="2" t="s">
@@ -2466,94 +2532,94 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="14">
         <v>5781</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="2" t="str">
+      <c r="E10" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="R10" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="S10" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="U10" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="V10" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="W10" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="Y10" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA10" s="2" t="str">
+      <c r="AA10" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep1</v>
       </c>
-      <c r="AB10" s="2" t="s">
+      <c r="AB10" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="AC10" s="13" t="s">
+      <c r="AC10" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2648,94 +2714,94 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="14">
         <v>5781</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="2" t="str">
+      <c r="E12" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U12" s="6" t="s">
+      <c r="U12" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="V12" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W12" s="6" t="s">
+      <c r="W12" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="X12" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y12" s="6" t="s">
+      <c r="Y12" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="Z12" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA12" s="2" t="str">
+      <c r="AA12" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB12" s="2" t="s">
+      <c r="AB12" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="AC12" s="13" t="s">
+      <c r="AC12" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2830,185 +2896,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="14">
         <v>7079</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="2" t="str">
+      <c r="E14" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N14" s="6" t="s">
+      <c r="H14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="R14" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S14" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U14" s="6" t="s">
+      <c r="U14" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="V14" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W14" s="6" t="s">
+      <c r="W14" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="X14" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y14" s="6" t="s">
+      <c r="Y14" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="Z14" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA14" s="2" t="str">
+      <c r="AA14" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSm2_day2_SS_rep1</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC14" s="13" t="s">
+        <v>r6-n_DSm2_day2_SS_rep2</v>
+      </c>
+      <c r="AB14" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC14" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="14">
         <v>5781</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="2" t="str">
+      <c r="E15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="R15" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="S15" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="T15" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U15" s="6" t="s">
+      <c r="U15" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="V15" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="W15" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="X15" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y15" s="6" t="s">
+      <c r="Y15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="Z15" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA15" s="2" t="str">
+      <c r="AA15" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB15" s="2" t="s">
+      <c r="AB15" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="AC15" s="13" t="s">
+      <c r="AC15" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3103,185 +3169,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="14">
         <v>7079</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="2" t="str">
+      <c r="E17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N17" s="6" t="s">
+      <c r="H17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="P17" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="R17" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="S17" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U17" s="6" t="s">
+      <c r="U17" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="V17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W17" s="6" t="s">
+      <c r="W17" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="X17" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y17" s="6" t="s">
+      <c r="Y17" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="Z17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA17" s="2" t="str">
+      <c r="AA17" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp2_day2_SS_rep1</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC17" s="13" t="s">
+        <v>r6-n_DSp2_day2_SS_rep2</v>
+      </c>
+      <c r="AB17" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC17" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="14">
         <v>5781</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="2" t="str">
+      <c r="E18" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="R18" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="S18" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U18" s="6" t="s">
+      <c r="U18" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V18" s="2" t="s">
+      <c r="V18" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W18" s="6" t="s">
+      <c r="W18" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="X18" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y18" s="6" t="s">
+      <c r="Y18" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="Z18" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA18" s="2" t="str">
+      <c r="AA18" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep1</v>
       </c>
-      <c r="AB18" s="2" t="s">
+      <c r="AB18" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="AC18" s="13" t="s">
+      <c r="AC18" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3376,185 +3442,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="14">
         <v>7079</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="2" t="str">
+      <c r="E20" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N20" s="6" t="s">
+      <c r="H20" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N20" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="O20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="P20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="Q20" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="R20" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S20" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U20" s="6" t="s">
+      <c r="U20" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="V20" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W20" s="6" t="s">
+      <c r="W20" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="X20" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y20" s="6" t="s">
+      <c r="Y20" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="Z20" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA20" s="2" t="str">
+      <c r="AA20" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp24_day3_SS_rep1</v>
-      </c>
-      <c r="AB20" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="AC20" s="13" t="s">
+        <v>r6-n_DSp24_day3_SS_rep2</v>
+      </c>
+      <c r="AB20" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC20" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="14">
         <v>5782</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="2" t="str">
+      <c r="E21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O21" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P21" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q21" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="R21" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="S21" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U21" s="6" t="s">
+      <c r="U21" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="V21" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W21" s="6" t="s">
+      <c r="W21" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="X21" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y21" s="6" t="s">
+      <c r="Y21" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="Z21" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA21" s="2" t="str">
+      <c r="AA21" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep2</v>
       </c>
-      <c r="AB21" s="2" t="s">
+      <c r="AB21" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="AC21" s="13" t="s">
+      <c r="AC21" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3649,185 +3715,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="14">
         <v>7078</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="2" t="str">
+      <c r="E23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N23" s="6" t="s">
+      <c r="H23" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N23" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="P23" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="Q23" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="R23" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="S23" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="T23" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U23" s="6" t="s">
+      <c r="U23" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="V23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W23" s="6" t="s">
+      <c r="W23" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X23" s="2" t="s">
+      <c r="X23" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y23" s="6" t="s">
+      <c r="Y23" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z23" s="2" t="s">
+      <c r="Z23" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA23" s="2" t="str">
+      <c r="AA23" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp48_day4_SS_rep2</v>
-      </c>
-      <c r="AB23" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AC23" s="13" t="s">
+        <v>r6-n_DSp48_day4_SS_rep1</v>
+      </c>
+      <c r="AB23" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="AC23" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="14">
         <v>5782</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="2" t="str">
+      <c r="E24" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P24" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="R24" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="S24" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T24" s="2" t="s">
+      <c r="T24" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U24" s="6" t="s">
+      <c r="U24" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="V24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W24" s="6" t="s">
+      <c r="W24" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X24" s="2" t="s">
+      <c r="X24" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y24" s="6" t="s">
+      <c r="Y24" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z24" s="2" t="s">
+      <c r="Z24" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA24" s="2" t="str">
+      <c r="AA24" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB24" s="2" t="s">
+      <c r="AB24" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="AC24" s="13" t="s">
+      <c r="AC24" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3922,185 +3988,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="14">
         <v>7078</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="2" t="str">
+      <c r="E26" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N26" s="6" t="s">
+      <c r="H26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O26" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q26" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="R26" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="S26" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="T26" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U26" s="6" t="s">
+      <c r="U26" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="V26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W26" s="6" t="s">
+      <c r="W26" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X26" s="2" t="s">
+      <c r="X26" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y26" s="6" t="s">
+      <c r="Y26" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z26" s="2" t="s">
+      <c r="Z26" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA26" s="2" t="str">
+      <c r="AA26" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSm2_day2_SS_rep2</v>
-      </c>
-      <c r="AB26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AC26" s="13" t="s">
+        <v>r6-n_DSm2_day2_SS_rep1</v>
+      </c>
+      <c r="AB26" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC26" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="14">
         <v>5782</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="2" t="str">
+      <c r="E27" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="O27" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="P27" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="Q27" s="2" t="s">
+      <c r="Q27" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="R27" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="S27" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="T27" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U27" s="6" t="s">
+      <c r="U27" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V27" s="2" t="s">
+      <c r="V27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W27" s="6" t="s">
+      <c r="W27" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X27" s="2" t="s">
+      <c r="X27" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y27" s="6" t="s">
+      <c r="Y27" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z27" s="2" t="s">
+      <c r="Z27" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA27" s="2" t="str">
+      <c r="AA27" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB27" s="2" t="s">
+      <c r="AB27" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="AC27" s="13" t="s">
+      <c r="AC27" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4195,185 +4261,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="14">
         <v>7078</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="2" t="str">
+      <c r="E29" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N29" s="6" t="s">
+      <c r="H29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="M29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N29" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="O29" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="P29" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="Q29" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="R29" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="S29" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="T29" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U29" s="6" t="s">
+      <c r="U29" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="V29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W29" s="6" t="s">
+      <c r="W29" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X29" s="2" t="s">
+      <c r="X29" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y29" s="6" t="s">
+      <c r="Y29" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z29" s="2" t="s">
+      <c r="Z29" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA29" s="2" t="str">
+      <c r="AA29" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp2_day2_SS_rep2</v>
-      </c>
-      <c r="AB29" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC29" s="13" t="s">
+        <v>r6-n_DSp2_day2_SS_rep1</v>
+      </c>
+      <c r="AB29" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="AC29" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="14">
         <v>5782</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="2" t="str">
+      <c r="E30" s="14" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M30" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N30" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="O30" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="P30" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="Q30" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="R30" s="2" t="s">
+      <c r="R30" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="S30" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="T30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U30" s="6" t="s">
+      <c r="U30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V30" s="2" t="s">
+      <c r="V30" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W30" s="6" t="s">
+      <c r="W30" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X30" s="2" t="s">
+      <c r="X30" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y30" s="6" t="s">
+      <c r="Y30" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z30" s="2" t="s">
+      <c r="Z30" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA30" s="2" t="str">
+      <c r="AA30" s="14" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB30" s="2" t="s">
+      <c r="AB30" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="AC30" s="13" t="s">
+      <c r="AC30" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4468,94 +4534,94 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="14">
         <v>7078</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="2" t="str">
+      <c r="E32" s="14" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="O32" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="2" t="s">
+      <c r="P32" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="Q32" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="R32" s="2" t="s">
+      <c r="R32" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="S32" s="2" t="s">
+      <c r="S32" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="T32" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U32" s="6" t="s">
+      <c r="U32" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V32" s="2" t="s">
+      <c r="V32" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W32" s="6" t="s">
+      <c r="W32" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X32" s="2" t="s">
+      <c r="X32" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y32" s="6" t="s">
+      <c r="Y32" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z32" s="2" t="s">
+      <c r="Z32" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AA32" s="2" t="str">
+      <c r="AA32" s="14" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB32" s="2" t="s">
+      <c r="AB32" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="AC32" s="13" t="s">
+      <c r="AC32" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6373,367 +6439,367 @@
         <v>369</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="14">
         <v>7078</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="2" t="str">
+      <c r="E53" s="14" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="J53" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="K53" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M53" s="2" t="s">
+      <c r="M53" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N53" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O53" s="2" t="s">
+      <c r="O53" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P53" s="2" t="s">
+      <c r="P53" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q53" s="2" t="s">
+      <c r="Q53" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="R53" s="2" t="s">
+      <c r="R53" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S53" s="2" t="s">
+      <c r="S53" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="T53" s="2" t="s">
+      <c r="T53" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U53" s="6" t="s">
+      <c r="U53" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V53" s="2" t="s">
+      <c r="V53" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W53" s="6" t="s">
+      <c r="W53" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X53" s="2" t="s">
+      <c r="X53" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y53" s="6" t="s">
+      <c r="Y53" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="Z53" s="2" t="s">
+      <c r="Z53" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AA53" s="2" t="str">
+      <c r="AA53" s="14" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep1</v>
       </c>
-      <c r="AB53" s="2" t="s">
+      <c r="AB53" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="AC53" s="13" t="s">
+      <c r="AC53" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="14">
         <v>7078</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="2" t="str">
+      <c r="E54" s="14" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="K54" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="M54" s="14" t="s">
         <v>71</v>
       </c>
       <c r="N54" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O54" s="2" t="s">
+      <c r="O54" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P54" s="2" t="s">
+      <c r="P54" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q54" s="2" t="s">
+      <c r="Q54" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="R54" s="2" t="s">
+      <c r="R54" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S54" s="2" t="s">
+      <c r="S54" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="T54" s="2" t="s">
+      <c r="T54" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U54" s="6" t="s">
+      <c r="U54" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V54" s="5" t="s">
+      <c r="V54" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="W54" s="9" t="s">
+      <c r="W54" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="X54" s="5" t="s">
+      <c r="X54" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="Y54" s="6" t="s">
+      <c r="Y54" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="Z54" s="2" t="s">
+      <c r="Z54" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AA54" s="2" t="str">
+      <c r="AA54" s="14" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep1</v>
       </c>
-      <c r="AB54" s="2" t="s">
+      <c r="AB54" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="AC54" s="13" t="s">
+      <c r="AC54" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="14">
         <v>7079</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="2" t="str">
+      <c r="E55" s="14" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="J55" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="K55" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="M55" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N55" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O55" s="2" t="s">
+      <c r="O55" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="2" t="s">
+      <c r="P55" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q55" s="2" t="s">
+      <c r="Q55" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="R55" s="2" t="s">
+      <c r="R55" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S55" s="2" t="s">
+      <c r="S55" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="T55" s="2" t="s">
+      <c r="T55" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U55" s="6" t="s">
+      <c r="U55" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V55" s="2" t="s">
+      <c r="V55" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="W55" s="6" t="s">
+      <c r="W55" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="X55" s="2" t="s">
+      <c r="X55" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Y55" s="6" t="s">
+      <c r="Y55" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="Z55" s="2" t="s">
+      <c r="Z55" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AA55" s="2" t="str">
+      <c r="AA55" s="14" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep2</v>
       </c>
-      <c r="AB55" s="2" t="s">
+      <c r="AB55" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="AC55" s="13" t="s">
+      <c r="AC55" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="14">
         <v>7079</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="2" t="str">
+      <c r="E56" s="14" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="14" t="s">
         <v>100</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="J56" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="K56" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="M56" s="14" t="s">
         <v>72</v>
       </c>
       <c r="N56" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O56" s="2" t="s">
+      <c r="O56" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P56" s="2" t="s">
+      <c r="P56" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q56" s="2" t="s">
+      <c r="Q56" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="R56" s="2" t="s">
+      <c r="R56" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S56" s="2" t="s">
+      <c r="S56" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="T56" s="2" t="s">
+      <c r="T56" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="U56" s="6" t="s">
+      <c r="U56" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V56" s="5" t="s">
+      <c r="V56" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="W56" s="9" t="s">
+      <c r="W56" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="X56" s="5" t="s">
+      <c r="X56" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="Y56" s="6" t="s">
+      <c r="Y56" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="Z56" s="2" t="s">
+      <c r="Z56" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AA56" s="2" t="str">
+      <c r="AA56" s="14" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep2</v>
       </c>
-      <c r="AB56" s="2" t="s">
+      <c r="AB56" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="AC56" s="13" t="s">
+      <c r="AC56" s="15" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6744,20 +6810,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6671224-CAF5-E647-BCC4-AFC80FBAC049}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -6818,7 +6883,7 @@
         <v>202</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f t="shared" ref="D3:D56" si="0">_xlfn.CONCAT(C3, E3)</f>
+        <f>_xlfn.CONCAT(C3, E3)</f>
         <v>WT_G1_day1_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -6842,7 +6907,7 @@
         <v>203</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C4, E4)</f>
         <v>WT_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -6866,7 +6931,7 @@
         <v>204</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C5, E5)</f>
         <v>WT_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -6890,7 +6955,7 @@
         <v>205</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C6, E6)</f>
         <v>WT_G1_day1_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -6914,7 +6979,7 @@
         <v>206</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C7, E7)</f>
         <v>WT_G1_day1_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -6938,7 +7003,7 @@
         <v>207</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C8, E8)</f>
         <v>WT_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -6962,7 +7027,7 @@
         <v>208</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C9, E9)</f>
         <v>WT_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -6986,7 +7051,7 @@
         <v>209</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C10, E10)</f>
         <v>WT_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -7010,7 +7075,7 @@
         <v>210</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C11, E11)</f>
         <v>t4-n_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -7034,7 +7099,7 @@
         <v>211</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C12, E12)</f>
         <v>WT_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -7058,7 +7123,7 @@
         <v>212</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C13, E13)</f>
         <v>t4-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -7079,11 +7144,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C14, E14)</f>
+        <v>r6-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>311</v>
@@ -7106,7 +7171,7 @@
         <v>214</v>
       </c>
       <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C15, E15)</f>
         <v>WT_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -7130,7 +7195,7 @@
         <v>215</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C16, E16)</f>
         <v>t4-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -7151,11 +7216,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C17, E17)</f>
+        <v>r6-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>311</v>
@@ -7178,7 +7243,7 @@
         <v>217</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C18, E18)</f>
         <v>WT_DSp24_day3_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -7202,7 +7267,7 @@
         <v>218</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C19, E19)</f>
         <v>t4-n_DSp24_day3_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -7223,11 +7288,11 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSp24_day3_SS_rep1.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C20, E20)</f>
+        <v>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>311</v>
@@ -7250,7 +7315,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C21, E21)</f>
         <v>WT_DSp48_day4_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -7274,7 +7339,7 @@
         <v>221</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C22, E22)</f>
         <v>t4-n_DSp48_day4_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -7295,11 +7360,11 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>222</v>
+        <v>379</v>
       </c>
       <c r="D23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSp48_day4_SS_rep2.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C23, E23)</f>
+        <v>r6-n_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>311</v>
@@ -7322,7 +7387,7 @@
         <v>223</v>
       </c>
       <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C24, E24)</f>
         <v>WT_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -7346,7 +7411,7 @@
         <v>224</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C25, E25)</f>
         <v>t4-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -7367,11 +7432,11 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C26, E26)</f>
+        <v>r6-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>311</v>
@@ -7394,7 +7459,7 @@
         <v>226</v>
       </c>
       <c r="D27" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C27, E27)</f>
         <v>WT_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -7418,7 +7483,7 @@
         <v>227</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C28, E28)</f>
         <v>t4-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -7439,11 +7504,11 @@
         <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>r6-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
+        <f>_xlfn.CONCAT(C29, E29)</f>
+        <v>r6-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>311</v>
@@ -7466,7 +7531,7 @@
         <v>229</v>
       </c>
       <c r="D30" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C30, E30)</f>
         <v>WT_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -7490,7 +7555,7 @@
         <v>230</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C31, E31)</f>
         <v>t4-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -7514,7 +7579,7 @@
         <v>231</v>
       </c>
       <c r="D32" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C32, E32)</f>
         <v>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -7538,7 +7603,7 @@
         <v>232</v>
       </c>
       <c r="D33" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C33, E33)</f>
         <v>n3-d_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -7562,7 +7627,7 @@
         <v>233</v>
       </c>
       <c r="D34" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C34, E34)</f>
         <v>n3-d_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -7586,7 +7651,7 @@
         <v>234</v>
       </c>
       <c r="D35" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C35, E35)</f>
         <v>o-d_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -7610,7 +7675,7 @@
         <v>235</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C36, E36)</f>
         <v>o-d_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -7634,7 +7699,7 @@
         <v>236</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C37, E37)</f>
         <v>o-d_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -7658,7 +7723,7 @@
         <v>237</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C38, E38)</f>
         <v>o-d_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -7682,7 +7747,7 @@
         <v>238</v>
       </c>
       <c r="D39" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C39, E39)</f>
         <v>n3-d_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -7706,7 +7771,7 @@
         <v>239</v>
       </c>
       <c r="D40" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C40, E40)</f>
         <v>n3-d_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -7730,7 +7795,7 @@
         <v>373</v>
       </c>
       <c r="D41" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C41, E41)</f>
         <v>n3-d_Q_day7_N_rep3.UTK_prim.bam</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -7754,7 +7819,7 @@
         <v>374</v>
       </c>
       <c r="D42" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C42, E42)</f>
         <v>n3-d_Q_day7_SS_rep3.UTK_prim.bam</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -7778,7 +7843,7 @@
         <v>371</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C43, E43)</f>
         <v>WT_Q_day7_N_rep2_CU.UTK_prim.bam</v>
       </c>
       <c r="E43" s="10" t="s">
@@ -7802,7 +7867,7 @@
         <v>372</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C44, E44)</f>
         <v>WT_Q_day7_SS_rep2_CU.UTK_prim.bam</v>
       </c>
       <c r="E44" s="10" t="s">
@@ -7826,7 +7891,7 @@
         <v>240</v>
       </c>
       <c r="D45" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C45, E45)</f>
         <v>r1-n_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -7850,7 +7915,7 @@
         <v>241</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C46, E46)</f>
         <v>r1-n_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -7874,7 +7939,7 @@
         <v>242</v>
       </c>
       <c r="D47" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C47, E47)</f>
         <v>r1-n_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -7898,7 +7963,7 @@
         <v>243</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C48, E48)</f>
         <v>r1-n_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -7922,7 +7987,7 @@
         <v>244</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C49, E49)</f>
         <v>WT_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -7946,7 +8011,7 @@
         <v>245</v>
       </c>
       <c r="D50" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C50, E50)</f>
         <v>WT_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -7970,7 +8035,7 @@
         <v>246</v>
       </c>
       <c r="D51" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C51, E51)</f>
         <v>WT_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -7994,7 +8059,7 @@
         <v>247</v>
       </c>
       <c r="D52" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C52, E52)</f>
         <v>WT_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -8018,7 +8083,7 @@
         <v>248</v>
       </c>
       <c r="D53" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C53, E53)</f>
         <v>r6-n_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -8042,7 +8107,7 @@
         <v>249</v>
       </c>
       <c r="D54" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C54, E54)</f>
         <v>r6-n_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -8066,7 +8131,7 @@
         <v>250</v>
       </c>
       <c r="D55" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C55, E55)</f>
         <v>r6-n_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -8090,7 +8155,7 @@
         <v>251</v>
       </c>
       <c r="D56" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C56, E56)</f>
         <v>r6-n_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -8102,6 +8167,171 @@
       <c r="G56" s="2" t="s">
         <v>362</v>
       </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="14"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="14"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="14"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="14"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="14"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="14"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="14"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="14"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="4"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" s="4"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="10"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="10"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C103" s="2"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C104" s="2"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C105" s="2"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="2"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="2"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="2"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="2"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C111" s="14"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="14"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C113" s="14"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C114" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G56">
@@ -8109,4 +8339,113 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082ED199-6BE6-DE4F-8415-858035711CE7}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="C3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work for 2023-0226: Correcting (minor) sample errors in counting features and beginning to do normalization (etc.) work
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4905C3AC-5DFB-3E4B-B281-D42EF9650B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48A854D-343E-7A40-B5E5-8BDA0BB0F887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7700" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -1212,6 +1212,7 @@
   <si>
     <r>
       <rPr>
+        <strike/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
@@ -1221,6 +1222,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -1229,13 +1231,30 @@
       </rPr>
       <t xml:space="preserve"> replace x-dekho with rep2; replace y-dekho with rep1</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Done.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1301,6 +1320,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1328,7 +1373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1343,11 +1388,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2532,94 +2574,94 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="2">
         <v>5781</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="14" t="str">
+      <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="T10" s="14" t="s">
+      <c r="T10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U10" s="14" t="s">
+      <c r="U10" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W10" s="14" t="s">
+      <c r="W10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X10" s="14" t="s">
+      <c r="X10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y10" s="14" t="s">
+      <c r="Y10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA10" s="14" t="str">
+      <c r="AA10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep1</v>
       </c>
-      <c r="AB10" s="14" t="s">
+      <c r="AB10" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AC10" s="15" t="s">
+      <c r="AC10" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2714,94 +2756,94 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="2">
         <v>5781</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="14" t="str">
+      <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S12" s="14" t="s">
+      <c r="S12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T12" s="14" t="s">
+      <c r="T12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U12" s="14" t="s">
+      <c r="U12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V12" s="14" t="s">
+      <c r="V12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W12" s="14" t="s">
+      <c r="W12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X12" s="14" t="s">
+      <c r="X12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y12" s="14" t="s">
+      <c r="Y12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z12" s="14" t="s">
+      <c r="Z12" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA12" s="14" t="str">
+      <c r="AA12" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB12" s="14" t="s">
+      <c r="AB12" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="AC12" s="15" t="s">
+      <c r="AC12" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2896,185 +2938,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="2">
         <v>7079</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="14" t="str">
+      <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="P14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R14" s="14" t="s">
+      <c r="R14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S14" s="14" t="s">
+      <c r="S14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T14" s="14" t="s">
+      <c r="T14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U14" s="14" t="s">
+      <c r="U14" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V14" s="14" t="s">
+      <c r="V14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W14" s="14" t="s">
+      <c r="W14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X14" s="14" t="s">
+      <c r="X14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y14" s="14" t="s">
+      <c r="Y14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z14" s="14" t="s">
+      <c r="Z14" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA14" s="14" t="str">
+      <c r="AA14" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB14" s="14" t="s">
+      <c r="AB14" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AC14" s="15" t="s">
+      <c r="AC14" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="2">
         <v>5781</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="14" t="str">
+      <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="O15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="P15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R15" s="14" t="s">
+      <c r="R15" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S15" s="14" t="s">
+      <c r="S15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U15" s="14" t="s">
+      <c r="U15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V15" s="14" t="s">
+      <c r="V15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W15" s="14" t="s">
+      <c r="W15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X15" s="14" t="s">
+      <c r="X15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y15" s="14" t="s">
+      <c r="Y15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z15" s="14" t="s">
+      <c r="Z15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA15" s="14" t="str">
+      <c r="AA15" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB15" s="14" t="s">
+      <c r="AB15" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AC15" s="15" t="s">
+      <c r="AC15" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3169,185 +3211,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="2">
         <v>7079</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="14" t="str">
+      <c r="E17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="S17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T17" s="14" t="s">
+      <c r="T17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U17" s="14" t="s">
+      <c r="U17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="V17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W17" s="14" t="s">
+      <c r="W17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X17" s="14" t="s">
+      <c r="X17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y17" s="14" t="s">
+      <c r="Y17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z17" s="14" t="s">
+      <c r="Z17" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA17" s="14" t="str">
+      <c r="AA17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB17" s="14" t="s">
+      <c r="AB17" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AC17" s="15" t="s">
+      <c r="AC17" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="2">
         <v>5781</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="14" t="str">
+      <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="P18" s="14" t="s">
+      <c r="P18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="R18" s="14" t="s">
+      <c r="R18" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="S18" s="14" t="s">
+      <c r="S18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T18" s="14" t="s">
+      <c r="T18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U18" s="14" t="s">
+      <c r="U18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V18" s="14" t="s">
+      <c r="V18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W18" s="14" t="s">
+      <c r="W18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X18" s="14" t="s">
+      <c r="X18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y18" s="14" t="s">
+      <c r="Y18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z18" s="14" t="s">
+      <c r="Z18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA18" s="14" t="str">
+      <c r="AA18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep1</v>
       </c>
-      <c r="AB18" s="14" t="s">
+      <c r="AB18" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AC18" s="15" t="s">
+      <c r="AC18" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3442,185 +3484,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="2">
         <v>7079</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="14" t="str">
+      <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="O20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="P20" s="14" t="s">
+      <c r="P20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" s="14" t="s">
+      <c r="Q20" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="14" t="s">
+      <c r="R20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="S20" s="14" t="s">
+      <c r="S20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T20" s="14" t="s">
+      <c r="T20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U20" s="14" t="s">
+      <c r="U20" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V20" s="14" t="s">
+      <c r="V20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W20" s="14" t="s">
+      <c r="W20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X20" s="14" t="s">
+      <c r="X20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y20" s="14" t="s">
+      <c r="Y20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z20" s="14" t="s">
+      <c r="Z20" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA20" s="14" t="str">
+      <c r="AA20" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB20" s="14" t="s">
+      <c r="AB20" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AC20" s="15" t="s">
+      <c r="AC20" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="2">
         <v>5782</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="14" t="str">
+      <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="O21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P21" s="14" t="s">
+      <c r="P21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q21" s="14" t="s">
+      <c r="Q21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="R21" s="14" t="s">
+      <c r="R21" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="S21" s="14" t="s">
+      <c r="S21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="T21" s="14" t="s">
+      <c r="T21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U21" s="14" t="s">
+      <c r="U21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V21" s="14" t="s">
+      <c r="V21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W21" s="14" t="s">
+      <c r="W21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X21" s="14" t="s">
+      <c r="X21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y21" s="14" t="s">
+      <c r="Y21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z21" s="14" t="s">
+      <c r="Z21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA21" s="14" t="str">
+      <c r="AA21" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_SS_rep2</v>
       </c>
-      <c r="AB21" s="14" t="s">
+      <c r="AB21" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AC21" s="15" t="s">
+      <c r="AC21" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3715,185 +3757,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="2">
         <v>7078</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="14" t="str">
+      <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="14" t="s">
+      <c r="O23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="P23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q23" s="14" t="s">
+      <c r="Q23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="14" t="s">
+      <c r="R23" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="S23" s="14" t="s">
+      <c r="S23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="T23" s="14" t="s">
+      <c r="T23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U23" s="14" t="s">
+      <c r="U23" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="V23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W23" s="14" t="s">
+      <c r="W23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X23" s="14" t="s">
+      <c r="X23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y23" s="14" t="s">
+      <c r="Y23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z23" s="14" t="s">
+      <c r="Z23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA23" s="14" t="str">
+      <c r="AA23" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp48_day4_SS_rep1</v>
       </c>
-      <c r="AB23" s="14" t="s">
+      <c r="AB23" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="AC23" s="15" t="s">
+      <c r="AC23" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="2">
         <v>5782</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="14" t="str">
+      <c r="E24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="O24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="P24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q24" s="14" t="s">
+      <c r="Q24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R24" s="14" t="s">
+      <c r="R24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S24" s="14" t="s">
+      <c r="S24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="T24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U24" s="14" t="s">
+      <c r="U24" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V24" s="14" t="s">
+      <c r="V24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W24" s="14" t="s">
+      <c r="W24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X24" s="14" t="s">
+      <c r="X24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y24" s="14" t="s">
+      <c r="Y24" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z24" s="14" t="s">
+      <c r="Z24" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA24" s="14" t="str">
+      <c r="AA24" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_SS_rep2</v>
       </c>
-      <c r="AB24" s="14" t="s">
+      <c r="AB24" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AC24" s="15" t="s">
+      <c r="AC24" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3988,185 +4030,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="2">
         <v>7078</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="14" t="str">
+      <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="O26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="P26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="Q26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R26" s="14" t="s">
+      <c r="R26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S26" s="14" t="s">
+      <c r="S26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T26" s="14" t="s">
+      <c r="T26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U26" s="14" t="s">
+      <c r="U26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="V26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W26" s="14" t="s">
+      <c r="W26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X26" s="14" t="s">
+      <c r="X26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y26" s="14" t="s">
+      <c r="Y26" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z26" s="14" t="s">
+      <c r="Z26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA26" s="14" t="str">
+      <c r="AA26" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSm2_day2_SS_rep1</v>
       </c>
-      <c r="AB26" s="14" t="s">
+      <c r="AB26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AC26" s="15" t="s">
+      <c r="AC26" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="2">
         <v>5782</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="14" t="str">
+      <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="14" t="s">
+      <c r="K27" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O27" s="14" t="s">
+      <c r="O27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P27" s="14" t="s">
+      <c r="P27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q27" s="14" t="s">
+      <c r="Q27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R27" s="14" t="s">
+      <c r="R27" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S27" s="14" t="s">
+      <c r="S27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T27" s="14" t="s">
+      <c r="T27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U27" s="14" t="s">
+      <c r="U27" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V27" s="14" t="s">
+      <c r="V27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W27" s="14" t="s">
+      <c r="W27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X27" s="14" t="s">
+      <c r="X27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y27" s="14" t="s">
+      <c r="Y27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z27" s="14" t="s">
+      <c r="Z27" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA27" s="14" t="str">
+      <c r="AA27" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_SS_rep2</v>
       </c>
-      <c r="AB27" s="14" t="s">
+      <c r="AB27" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AC27" s="15" t="s">
+      <c r="AC27" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4261,185 +4303,185 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="2">
         <v>7078</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="14" t="str">
+      <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K29" s="14" t="s">
+      <c r="K29" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L29" s="14" t="s">
+      <c r="L29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N29" s="14" t="s">
+      <c r="N29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O29" s="14" t="s">
+      <c r="O29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P29" s="14" t="s">
+      <c r="P29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q29" s="14" t="s">
+      <c r="Q29" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R29" s="14" t="s">
+      <c r="R29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="S29" s="14" t="s">
+      <c r="S29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T29" s="14" t="s">
+      <c r="T29" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U29" s="14" t="s">
+      <c r="U29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V29" s="14" t="s">
+      <c r="V29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W29" s="14" t="s">
+      <c r="W29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X29" s="14" t="s">
+      <c r="X29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y29" s="14" t="s">
+      <c r="Y29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z29" s="14" t="s">
+      <c r="Z29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA29" s="14" t="str">
+      <c r="AA29" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp2_day2_SS_rep1</v>
       </c>
-      <c r="AB29" s="14" t="s">
+      <c r="AB29" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AC29" s="15" t="s">
+      <c r="AC29" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="2">
         <v>5782</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="14" t="str">
+      <c r="E30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="14" t="s">
+      <c r="K30" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="M30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N30" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O30" s="14" t="s">
+      <c r="O30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="P30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="14" t="s">
+      <c r="Q30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="R30" s="14" t="s">
+      <c r="R30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="S30" s="14" t="s">
+      <c r="S30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T30" s="14" t="s">
+      <c r="T30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U30" s="14" t="s">
+      <c r="U30" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V30" s="14" t="s">
+      <c r="V30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W30" s="14" t="s">
+      <c r="W30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X30" s="14" t="s">
+      <c r="X30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y30" s="14" t="s">
+      <c r="Y30" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z30" s="14" t="s">
+      <c r="Z30" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA30" s="14" t="str">
+      <c r="AA30" s="2" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB30" s="14" t="s">
+      <c r="AB30" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="AC30" s="15" t="s">
+      <c r="AC30" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4534,94 +4576,94 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="2">
         <v>7078</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="14" t="str">
+      <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="O32" s="14" t="s">
+      <c r="O32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="14" t="s">
+      <c r="P32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" s="14" t="s">
+      <c r="Q32" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="R32" s="14" t="s">
+      <c r="R32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="S32" s="14" t="s">
+      <c r="S32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T32" s="14" t="s">
+      <c r="T32" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U32" s="14" t="s">
+      <c r="U32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V32" s="14" t="s">
+      <c r="V32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W32" s="14" t="s">
+      <c r="W32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X32" s="14" t="s">
+      <c r="X32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y32" s="14" t="s">
+      <c r="Y32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Z32" s="14" t="s">
+      <c r="Z32" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AA32" s="14" t="str">
+      <c r="AA32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_DSp24_day3_SS_rep2</v>
       </c>
-      <c r="AB32" s="14" t="s">
+      <c r="AB32" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AC32" s="15" t="s">
+      <c r="AC32" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6439,367 +6481,367 @@
         <v>369</v>
       </c>
     </row>
-    <row r="53" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="2">
         <v>7078</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="14" t="str">
+      <c r="E53" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H53" s="14" t="s">
+      <c r="H53" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J53" s="14" t="s">
+      <c r="J53" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K53" s="14" t="s">
+      <c r="K53" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M53" s="14" t="s">
+      <c r="M53" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N53" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O53" s="14" t="s">
+      <c r="O53" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P53" s="14" t="s">
+      <c r="P53" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q53" s="14" t="s">
+      <c r="Q53" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="R53" s="14" t="s">
+      <c r="R53" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S53" s="14" t="s">
+      <c r="S53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T53" s="14" t="s">
+      <c r="T53" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U53" s="14" t="s">
+      <c r="U53" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V53" s="14" t="s">
+      <c r="V53" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W53" s="14" t="s">
+      <c r="W53" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X53" s="14" t="s">
+      <c r="X53" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y53" s="14" t="s">
+      <c r="Y53" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Z53" s="14" t="s">
+      <c r="Z53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AA53" s="14" t="str">
+      <c r="AA53" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep1</v>
       </c>
-      <c r="AB53" s="14" t="s">
+      <c r="AB53" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AC53" s="15" t="s">
+      <c r="AC53" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="2">
         <v>7078</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="14" t="str">
+      <c r="E54" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J54" s="14" t="s">
+      <c r="J54" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K54" s="14" t="s">
+      <c r="K54" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M54" s="14" t="s">
+      <c r="M54" s="2" t="s">
         <v>71</v>
       </c>
       <c r="N54" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O54" s="14" t="s">
+      <c r="O54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P54" s="14" t="s">
+      <c r="P54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q54" s="14" t="s">
+      <c r="Q54" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="R54" s="14" t="s">
+      <c r="R54" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S54" s="14" t="s">
+      <c r="S54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T54" s="14" t="s">
+      <c r="T54" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U54" s="14" t="s">
+      <c r="U54" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V54" s="17" t="s">
+      <c r="V54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W54" s="17" t="s">
+      <c r="W54" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="X54" s="17" t="s">
+      <c r="X54" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="Y54" s="14" t="s">
+      <c r="Y54" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Z54" s="14" t="s">
+      <c r="Z54" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AA54" s="14" t="str">
+      <c r="AA54" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep1</v>
       </c>
-      <c r="AB54" s="14" t="s">
+      <c r="AB54" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AC54" s="15" t="s">
+      <c r="AC54" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="2">
         <v>7079</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="14" t="str">
+      <c r="E55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J55" s="14" t="s">
+      <c r="J55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K55" s="14" t="s">
+      <c r="K55" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M55" s="14" t="s">
+      <c r="M55" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N55" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O55" s="14" t="s">
+      <c r="O55" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="14" t="s">
+      <c r="P55" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q55" s="14" t="s">
+      <c r="Q55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="R55" s="14" t="s">
+      <c r="R55" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S55" s="14" t="s">
+      <c r="S55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T55" s="14" t="s">
+      <c r="T55" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U55" s="14" t="s">
+      <c r="U55" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V55" s="14" t="s">
+      <c r="V55" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W55" s="14" t="s">
+      <c r="W55" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X55" s="14" t="s">
+      <c r="X55" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y55" s="14" t="s">
+      <c r="Y55" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Z55" s="14" t="s">
+      <c r="Z55" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AA55" s="14" t="str">
+      <c r="AA55" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep2</v>
       </c>
-      <c r="AB55" s="14" t="s">
+      <c r="AB55" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="AC55" s="15" t="s">
+      <c r="AC55" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="2">
         <v>7079</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="14" t="str">
+      <c r="E56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rrp6-null</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="J56" s="14" t="s">
+      <c r="J56" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K56" s="14" t="s">
+      <c r="K56" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M56" s="14" t="s">
+      <c r="M56" s="2" t="s">
         <v>72</v>
       </c>
       <c r="N56" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O56" s="14" t="s">
+      <c r="O56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P56" s="14" t="s">
+      <c r="P56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q56" s="14" t="s">
+      <c r="Q56" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="R56" s="14" t="s">
+      <c r="R56" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S56" s="14" t="s">
+      <c r="S56" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T56" s="14" t="s">
+      <c r="T56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U56" s="14" t="s">
+      <c r="U56" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V56" s="17" t="s">
+      <c r="V56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W56" s="17" t="s">
+      <c r="W56" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="X56" s="17" t="s">
+      <c r="X56" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="Y56" s="14" t="s">
+      <c r="Y56" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Z56" s="14" t="s">
+      <c r="Z56" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AA56" s="14" t="str">
+      <c r="AA56" s="2" t="str">
         <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep2</v>
       </c>
-      <c r="AB56" s="14" t="s">
+      <c r="AB56" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AC56" s="15" t="s">
+      <c r="AC56" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6812,7 +6854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6671224-CAF5-E647-BCC4-AFC80FBAC049}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6859,7 +6901,7 @@
         <v>201</v>
       </c>
       <c r="D2" s="2" t="str">
-        <f>_xlfn.CONCAT(C2, E2)</f>
+        <f t="shared" ref="D2:D33" si="0">_xlfn.CONCAT(C2, E2)</f>
         <v>WT_G1_day1_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -6883,7 +6925,7 @@
         <v>202</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f>_xlfn.CONCAT(C3, E3)</f>
+        <f t="shared" si="0"/>
         <v>WT_G1_day1_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -6907,7 +6949,7 @@
         <v>203</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f>_xlfn.CONCAT(C4, E4)</f>
+        <f t="shared" si="0"/>
         <v>WT_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -6931,7 +6973,7 @@
         <v>204</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>_xlfn.CONCAT(C5, E5)</f>
+        <f t="shared" si="0"/>
         <v>WT_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -6955,7 +6997,7 @@
         <v>205</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>_xlfn.CONCAT(C6, E6)</f>
+        <f t="shared" si="0"/>
         <v>WT_G1_day1_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -6979,7 +7021,7 @@
         <v>206</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f>_xlfn.CONCAT(C7, E7)</f>
+        <f t="shared" si="0"/>
         <v>WT_G1_day1_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -7003,7 +7045,7 @@
         <v>207</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>_xlfn.CONCAT(C8, E8)</f>
+        <f t="shared" si="0"/>
         <v>WT_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -7027,7 +7069,7 @@
         <v>208</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>_xlfn.CONCAT(C9, E9)</f>
+        <f t="shared" si="0"/>
         <v>WT_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -7051,7 +7093,7 @@
         <v>209</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>_xlfn.CONCAT(C10, E10)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -7075,7 +7117,7 @@
         <v>210</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>_xlfn.CONCAT(C11, E11)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -7099,7 +7141,7 @@
         <v>211</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>_xlfn.CONCAT(C12, E12)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -7123,7 +7165,7 @@
         <v>212</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>_xlfn.CONCAT(C13, E13)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -7147,7 +7189,7 @@
         <v>225</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f>_xlfn.CONCAT(C14, E14)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -7171,7 +7213,7 @@
         <v>214</v>
       </c>
       <c r="D15" s="2" t="str">
-        <f>_xlfn.CONCAT(C15, E15)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -7195,7 +7237,7 @@
         <v>215</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>_xlfn.CONCAT(C16, E16)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -7219,7 +7261,7 @@
         <v>228</v>
       </c>
       <c r="D17" s="2" t="str">
-        <f>_xlfn.CONCAT(C17, E17)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -7243,7 +7285,7 @@
         <v>217</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f>_xlfn.CONCAT(C18, E18)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp24_day3_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -7267,7 +7309,7 @@
         <v>218</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f>_xlfn.CONCAT(C19, E19)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp24_day3_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -7291,7 +7333,7 @@
         <v>231</v>
       </c>
       <c r="D20" s="2" t="str">
-        <f>_xlfn.CONCAT(C20, E20)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -7315,7 +7357,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f>_xlfn.CONCAT(C21, E21)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp48_day4_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -7339,7 +7381,7 @@
         <v>221</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>_xlfn.CONCAT(C22, E22)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp48_day4_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -7363,7 +7405,7 @@
         <v>379</v>
       </c>
       <c r="D23" s="2" t="str">
-        <f>_xlfn.CONCAT(C23, E23)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSp48_day4_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -7387,7 +7429,7 @@
         <v>223</v>
       </c>
       <c r="D24" s="2" t="str">
-        <f>_xlfn.CONCAT(C24, E24)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -7411,7 +7453,7 @@
         <v>224</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>_xlfn.CONCAT(C25, E25)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSm2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -7435,7 +7477,7 @@
         <v>213</v>
       </c>
       <c r="D26" s="2" t="str">
-        <f>_xlfn.CONCAT(C26, E26)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSm2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -7459,7 +7501,7 @@
         <v>226</v>
       </c>
       <c r="D27" s="2" t="str">
-        <f>_xlfn.CONCAT(C27, E27)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -7483,7 +7525,7 @@
         <v>227</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>_xlfn.CONCAT(C28, E28)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp2_day2_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -7507,7 +7549,7 @@
         <v>216</v>
       </c>
       <c r="D29" s="2" t="str">
-        <f>_xlfn.CONCAT(C29, E29)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSp2_day2_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -7531,7 +7573,7 @@
         <v>229</v>
       </c>
       <c r="D30" s="2" t="str">
-        <f>_xlfn.CONCAT(C30, E30)</f>
+        <f t="shared" si="0"/>
         <v>WT_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -7555,7 +7597,7 @@
         <v>230</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>_xlfn.CONCAT(C31, E31)</f>
+        <f t="shared" si="0"/>
         <v>t4-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -7579,7 +7621,7 @@
         <v>231</v>
       </c>
       <c r="D32" s="2" t="str">
-        <f>_xlfn.CONCAT(C32, E32)</f>
+        <f t="shared" si="0"/>
         <v>r6-n_DSp24_day3_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -7603,7 +7645,7 @@
         <v>232</v>
       </c>
       <c r="D33" s="4" t="str">
-        <f>_xlfn.CONCAT(C33, E33)</f>
+        <f t="shared" si="0"/>
         <v>n3-d_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -7627,7 +7669,7 @@
         <v>233</v>
       </c>
       <c r="D34" s="4" t="str">
-        <f>_xlfn.CONCAT(C34, E34)</f>
+        <f t="shared" ref="D34:D65" si="1">_xlfn.CONCAT(C34, E34)</f>
         <v>n3-d_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -7651,7 +7693,7 @@
         <v>234</v>
       </c>
       <c r="D35" s="2" t="str">
-        <f>_xlfn.CONCAT(C35, E35)</f>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -7675,7 +7717,7 @@
         <v>235</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f>_xlfn.CONCAT(C36, E36)</f>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -7699,7 +7741,7 @@
         <v>236</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f>_xlfn.CONCAT(C37, E37)</f>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -7723,7 +7765,7 @@
         <v>237</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>_xlfn.CONCAT(C38, E38)</f>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -7747,7 +7789,7 @@
         <v>238</v>
       </c>
       <c r="D39" s="4" t="str">
-        <f>_xlfn.CONCAT(C39, E39)</f>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -7771,7 +7813,7 @@
         <v>239</v>
       </c>
       <c r="D40" s="4" t="str">
-        <f>_xlfn.CONCAT(C40, E40)</f>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -7795,7 +7837,7 @@
         <v>373</v>
       </c>
       <c r="D41" s="4" t="str">
-        <f>_xlfn.CONCAT(C41, E41)</f>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_N_rep3.UTK_prim.bam</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -7819,7 +7861,7 @@
         <v>374</v>
       </c>
       <c r="D42" s="4" t="str">
-        <f>_xlfn.CONCAT(C42, E42)</f>
+        <f t="shared" si="1"/>
         <v>n3-d_Q_day7_SS_rep3.UTK_prim.bam</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -7843,7 +7885,7 @@
         <v>371</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f>_xlfn.CONCAT(C43, E43)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_N_rep2_CU.UTK_prim.bam</v>
       </c>
       <c r="E43" s="10" t="s">
@@ -7867,7 +7909,7 @@
         <v>372</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f>_xlfn.CONCAT(C44, E44)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day7_SS_rep2_CU.UTK_prim.bam</v>
       </c>
       <c r="E44" s="10" t="s">
@@ -7891,7 +7933,7 @@
         <v>240</v>
       </c>
       <c r="D45" s="2" t="str">
-        <f>_xlfn.CONCAT(C45, E45)</f>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -7915,7 +7957,7 @@
         <v>241</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f>_xlfn.CONCAT(C46, E46)</f>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -7939,7 +7981,7 @@
         <v>242</v>
       </c>
       <c r="D47" s="2" t="str">
-        <f>_xlfn.CONCAT(C47, E47)</f>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -7963,7 +8005,7 @@
         <v>243</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f>_xlfn.CONCAT(C48, E48)</f>
+        <f t="shared" si="1"/>
         <v>r1-n_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -7987,7 +8029,7 @@
         <v>244</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f>_xlfn.CONCAT(C49, E49)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -8011,7 +8053,7 @@
         <v>245</v>
       </c>
       <c r="D50" s="2" t="str">
-        <f>_xlfn.CONCAT(C50, E50)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -8035,7 +8077,7 @@
         <v>246</v>
       </c>
       <c r="D51" s="2" t="str">
-        <f>_xlfn.CONCAT(C51, E51)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -8059,7 +8101,7 @@
         <v>247</v>
       </c>
       <c r="D52" s="2" t="str">
-        <f>_xlfn.CONCAT(C52, E52)</f>
+        <f t="shared" si="1"/>
         <v>WT_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -8083,7 +8125,7 @@
         <v>248</v>
       </c>
       <c r="D53" s="2" t="str">
-        <f>_xlfn.CONCAT(C53, E53)</f>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep1.UTK_prim.bam</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -8107,7 +8149,7 @@
         <v>249</v>
       </c>
       <c r="D54" s="2" t="str">
-        <f>_xlfn.CONCAT(C54, E54)</f>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep1.UTK_prim.bam</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -8131,7 +8173,7 @@
         <v>250</v>
       </c>
       <c r="D55" s="2" t="str">
-        <f>_xlfn.CONCAT(C55, E55)</f>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_SS_rep2.UTK_prim.bam</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -8155,7 +8197,7 @@
         <v>251</v>
       </c>
       <c r="D56" s="2" t="str">
-        <f>_xlfn.CONCAT(C56, E56)</f>
+        <f t="shared" si="1"/>
         <v>r6-n_Q_day8_N_rep2.UTK_prim.bam</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -8193,73 +8235,73 @@
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="14"/>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="14"/>
+      <c r="C70" s="2"/>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" s="3"/>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="14"/>
+      <c r="C72" s="2"/>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="14"/>
+      <c r="C73" s="2"/>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="3"/>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="14"/>
+      <c r="C75" s="2"/>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C76" s="14"/>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C78" s="14"/>
+      <c r="C78" s="2"/>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C79" s="14"/>
+      <c r="C79" s="2"/>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="3"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="14"/>
+      <c r="C81" s="2"/>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="14"/>
+      <c r="C82" s="2"/>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="3"/>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="14"/>
+      <c r="C84" s="2"/>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="14"/>
+      <c r="C85" s="2"/>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="3"/>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" s="14"/>
+      <c r="C87" s="2"/>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" s="14"/>
+      <c r="C88" s="2"/>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="14"/>
+      <c r="C90" s="2"/>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="4"/>
@@ -8322,16 +8364,16 @@
       <c r="C110" s="2"/>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C111" s="14"/>
+      <c r="C111" s="2"/>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C112" s="14"/>
+      <c r="C112" s="2"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C113" s="14"/>
+      <c r="C113" s="2"/>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C114" s="14"/>
+      <c r="C114" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G56">
@@ -8345,7 +8387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082ED199-6BE6-DE4F-8415-858035711CE7}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8364,15 +8406,15 @@
       <c r="C1" t="s">
         <v>381</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>383</v>
       </c>
       <c r="C2" t="s">
@@ -8380,10 +8422,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>384</v>
       </c>
       <c r="C3" t="s">
@@ -8391,10 +8433,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>385</v>
       </c>
       <c r="C4" t="s">
@@ -8402,10 +8444,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>386</v>
       </c>
       <c r="C5" t="s">
@@ -8413,10 +8455,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>387</v>
       </c>
       <c r="C6" t="s">
@@ -8424,10 +8466,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>388</v>
       </c>
       <c r="C7" t="s">
@@ -8435,10 +8477,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>389</v>
       </c>
       <c r="C8" t="s">

</xml_diff>

<commit_message>
Work for 2023-0307 and the morning of 2023-0308: NNS comparisons and size-factor estimation tests
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD2E2BE-9C96-B74D-83D7-F542BE8AE4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCE704A-7584-6545-B5EB-324AB59656A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>aux-T</t>
-  </si>
-  <si>
-    <t>Ostir-depletion</t>
   </si>
   <si>
     <t>o-d</t>
@@ -734,6 +731,9 @@
   </si>
   <si>
     <t>ovn</t>
+  </si>
+  <si>
+    <t>OsTIR-depletion</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -867,12 +867,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,42 +1190,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D52A0-EFB8-324D-84A5-D98AF0E44661}">
   <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W26" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AD39" sqref="AD39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="40.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -1237,7 +1232,7 @@
         <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>94</v>
@@ -1252,25 +1247,25 @@
         <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>57</v>
@@ -1279,13 +1274,13 @@
         <v>90</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>91</v>
@@ -1293,8 +1288,8 @@
       <c r="T1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="17" t="s">
-        <v>128</v>
+      <c r="U1" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>62</v>
@@ -1309,13 +1304,13 @@
         <v>65</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>70</v>
@@ -1326,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1">
         <v>5781</v>
@@ -1339,16 +1334,16 @@
         <v>wild-type</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>71</v>
@@ -1357,7 +1352,7 @@
         <v>95</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>71</v>
@@ -1369,13 +1364,13 @@
         <v>58</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>80</v>
@@ -1383,8 +1378,8 @@
       <c r="T2" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U2" s="17" t="s">
-        <v>129</v>
+      <c r="U2" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>63</v>
@@ -1399,13 +1394,13 @@
         <v>98</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC2" s="1" t="str">
         <f>_xlfn.CONCAT(F2, "_", N2, "_", R2, "_", AB2, "_", W2, "_",  T2, "_", Y2, "_", I2)</f>
@@ -1417,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="1">
         <v>5781</v>
@@ -1430,16 +1425,16 @@
         <v>wild-type</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>71</v>
@@ -1448,7 +1443,7 @@
         <v>95</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>71</v>
@@ -1460,13 +1455,13 @@
         <v>58</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>80</v>
@@ -1474,8 +1469,8 @@
       <c r="T3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U3" s="17" t="s">
-        <v>129</v>
+      <c r="U3" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>64</v>
@@ -1490,16 +1485,16 @@
         <v>98</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC3" s="1" t="str">
-        <f t="shared" ref="AC3:AC38" si="1">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", AB3, "_", W3, "_",  T3, "_", Y3, "_", I3)</f>
+        <f t="shared" ref="AC3:AC37" si="1">_xlfn.CONCAT(F3, "_", N3, "_", R3, "_", AB3, "_", W3, "_",  T3, "_", Y3, "_", I3)</f>
         <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep1</v>
       </c>
     </row>
@@ -1508,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="1">
         <v>5781</v>
@@ -1521,16 +1516,16 @@
         <v>wild-type</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>71</v>
@@ -1539,7 +1534,7 @@
         <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>71</v>
@@ -1557,7 +1552,7 @@
         <v>99</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>81</v>
@@ -1565,8 +1560,8 @@
       <c r="T4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U4" s="17" t="s">
-        <v>129</v>
+      <c r="U4" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>63</v>
@@ -1581,13 +1576,13 @@
         <v>98</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC4" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1599,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1">
         <v>5781</v>
@@ -1612,16 +1607,16 @@
         <v>wild-type</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>71</v>
@@ -1630,7 +1625,7 @@
         <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>71</v>
@@ -1648,7 +1643,7 @@
         <v>99</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>81</v>
@@ -1656,8 +1651,8 @@
       <c r="T5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U5" s="17" t="s">
-        <v>129</v>
+      <c r="U5" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>64</v>
@@ -1672,13 +1667,13 @@
         <v>98</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1690,7 +1685,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="1">
         <v>5782</v>
@@ -1703,16 +1698,16 @@
         <v>wild-type</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>72</v>
@@ -1721,7 +1716,7 @@
         <v>100</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>72</v>
@@ -1733,13 +1728,13 @@
         <v>58</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>80</v>
@@ -1747,8 +1742,8 @@
       <c r="T6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U6" s="17" t="s">
-        <v>129</v>
+      <c r="U6" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>63</v>
@@ -1763,13 +1758,13 @@
         <v>98</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC6" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1781,7 +1776,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1">
         <v>5782</v>
@@ -1794,16 +1789,16 @@
         <v>wild-type</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>72</v>
@@ -1812,7 +1807,7 @@
         <v>100</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>72</v>
@@ -1824,13 +1819,13 @@
         <v>58</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>80</v>
@@ -1838,8 +1833,8 @@
       <c r="T7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U7" s="17" t="s">
-        <v>129</v>
+      <c r="U7" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>64</v>
@@ -1854,13 +1849,13 @@
         <v>98</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC7" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1872,7 +1867,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="1">
         <v>5782</v>
@@ -1885,16 +1880,16 @@
         <v>wild-type</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>72</v>
@@ -1903,7 +1898,7 @@
         <v>100</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>72</v>
@@ -1921,7 +1916,7 @@
         <v>99</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>81</v>
@@ -1929,8 +1924,8 @@
       <c r="T8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U8" s="17" t="s">
-        <v>129</v>
+      <c r="U8" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>63</v>
@@ -1945,13 +1940,13 @@
         <v>98</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1963,7 +1958,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="1">
         <v>5782</v>
@@ -1976,16 +1971,16 @@
         <v>wild-type</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>72</v>
@@ -1994,7 +1989,7 @@
         <v>100</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>72</v>
@@ -2012,7 +2007,7 @@
         <v>99</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>81</v>
@@ -2020,8 +2015,8 @@
       <c r="T9" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U9" s="17" t="s">
-        <v>129</v>
+      <c r="U9" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>64</v>
@@ -2036,13 +2031,13 @@
         <v>98</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2054,7 +2049,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1">
         <v>5781</v>
@@ -2067,16 +2062,16 @@
         <v>wild-type</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>71</v>
@@ -2085,7 +2080,7 @@
         <v>95</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>71</v>
@@ -2103,7 +2098,7 @@
         <v>101</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>82</v>
@@ -2111,8 +2106,8 @@
       <c r="T10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U10" s="17" t="s">
-        <v>129</v>
+      <c r="U10" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>63</v>
@@ -2127,25 +2122,25 @@
         <v>102</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="2">
         <v>7080</v>
@@ -2161,13 +2156,13 @@
         <v>104</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>71</v>
@@ -2176,7 +2171,7 @@
         <v>95</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>71</v>
@@ -2194,7 +2189,7 @@
         <v>101</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>82</v>
@@ -2202,8 +2197,8 @@
       <c r="T11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U11" s="18" t="s">
-        <v>129</v>
+      <c r="U11" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>63</v>
@@ -2218,13 +2213,13 @@
         <v>102</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2236,7 +2231,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="1">
         <v>5781</v>
@@ -2249,16 +2244,16 @@
         <v>wild-type</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>71</v>
@@ -2267,7 +2262,7 @@
         <v>95</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>71</v>
@@ -2285,7 +2280,7 @@
         <v>105</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>83</v>
@@ -2293,8 +2288,8 @@
       <c r="T12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U12" s="17" t="s">
-        <v>129</v>
+      <c r="U12" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>63</v>
@@ -2309,25 +2304,25 @@
         <v>102</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="2">
         <v>7080</v>
@@ -2343,13 +2338,13 @@
         <v>104</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>71</v>
@@ -2358,7 +2353,7 @@
         <v>95</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>71</v>
@@ -2376,7 +2371,7 @@
         <v>105</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>83</v>
@@ -2384,8 +2379,8 @@
       <c r="T13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U13" s="18" t="s">
-        <v>129</v>
+      <c r="U13" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V13" s="2" t="s">
         <v>63</v>
@@ -2400,13 +2395,13 @@
         <v>102</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2418,7 +2413,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" s="1">
         <v>7079</v>
@@ -2434,13 +2429,13 @@
         <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>72</v>
@@ -2449,7 +2444,7 @@
         <v>100</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>72</v>
@@ -2467,7 +2462,7 @@
         <v>105</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>83</v>
@@ -2475,8 +2470,8 @@
       <c r="T14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U14" s="17" t="s">
-        <v>129</v>
+      <c r="U14" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>63</v>
@@ -2491,13 +2486,13 @@
         <v>102</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC14" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2509,7 +2504,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="1">
         <v>5781</v>
@@ -2522,16 +2517,16 @@
         <v>wild-type</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>71</v>
@@ -2540,7 +2535,7 @@
         <v>95</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>71</v>
@@ -2558,7 +2553,7 @@
         <v>105</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>83</v>
@@ -2566,8 +2561,8 @@
       <c r="T15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U15" s="17" t="s">
-        <v>129</v>
+      <c r="U15" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>63</v>
@@ -2582,25 +2577,25 @@
         <v>102</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2">
         <v>7080</v>
@@ -2616,13 +2611,13 @@
         <v>104</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>71</v>
@@ -2631,7 +2626,7 @@
         <v>95</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>71</v>
@@ -2649,7 +2644,7 @@
         <v>105</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>83</v>
@@ -2657,8 +2652,8 @@
       <c r="T16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U16" s="18" t="s">
-        <v>129</v>
+      <c r="U16" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>63</v>
@@ -2673,13 +2668,13 @@
         <v>102</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2691,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="1">
         <v>7079</v>
@@ -2707,13 +2702,13 @@
         <v>107</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>72</v>
@@ -2722,7 +2717,7 @@
         <v>100</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>72</v>
@@ -2740,7 +2735,7 @@
         <v>105</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>83</v>
@@ -2748,8 +2743,8 @@
       <c r="T17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U17" s="17" t="s">
-        <v>129</v>
+      <c r="U17" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>63</v>
@@ -2764,13 +2759,13 @@
         <v>102</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2782,7 +2777,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="1">
         <v>5781</v>
@@ -2795,16 +2790,16 @@
         <v>wild-type</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>71</v>
@@ -2813,7 +2808,7 @@
         <v>95</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>71</v>
@@ -2831,7 +2826,7 @@
         <v>108</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>84</v>
@@ -2839,8 +2834,8 @@
       <c r="T18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U18" s="17" t="s">
-        <v>129</v>
+      <c r="U18" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>63</v>
@@ -2855,25 +2850,25 @@
         <v>102</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="2">
         <v>7080</v>
@@ -2889,13 +2884,13 @@
         <v>104</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>71</v>
@@ -2904,7 +2899,7 @@
         <v>95</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>71</v>
@@ -2922,7 +2917,7 @@
         <v>108</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>84</v>
@@ -2930,8 +2925,8 @@
       <c r="T19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U19" s="18" t="s">
-        <v>129</v>
+      <c r="U19" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V19" s="2" t="s">
         <v>63</v>
@@ -2946,13 +2941,13 @@
         <v>102</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2960,90 +2955,90 @@
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="C20" s="17">
+      <c r="B20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="1">
         <v>7079</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="17" t="str">
+      <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H20" s="17" t="s">
+      <c r="G20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="J20" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="M20" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>72</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P20" s="17" t="s">
+      <c r="P20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" s="17" t="s">
+      <c r="Q20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="S20" s="17" t="s">
+      <c r="R20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U20" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="V20" s="17" t="s">
+      <c r="U20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V20" s="1" t="s">
         <v>63</v>
       </c>
       <c r="W20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="X20" s="17" t="s">
+      <c r="X20" s="1" t="s">
         <v>88</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="Z20" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA20" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB20" s="17" t="s">
-        <v>218</v>
+      <c r="Z20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="AC20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3055,7 +3050,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" s="1">
         <v>5782</v>
@@ -3068,16 +3063,16 @@
         <v>wild-type</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
@@ -3086,7 +3081,7 @@
         <v>100</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>72</v>
@@ -3104,7 +3099,7 @@
         <v>101</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>82</v>
@@ -3112,8 +3107,8 @@
       <c r="T21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U21" s="17" t="s">
-        <v>129</v>
+      <c r="U21" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>63</v>
@@ -3128,25 +3123,25 @@
         <v>102</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="2">
         <v>7081</v>
@@ -3162,13 +3157,13 @@
         <v>104</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>72</v>
@@ -3177,7 +3172,7 @@
         <v>100</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>72</v>
@@ -3195,7 +3190,7 @@
         <v>101</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>82</v>
@@ -3203,8 +3198,8 @@
       <c r="T22" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U22" s="18" t="s">
-        <v>129</v>
+      <c r="U22" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>63</v>
@@ -3219,13 +3214,13 @@
         <v>102</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3237,7 +3232,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="1">
         <v>7078</v>
@@ -3253,13 +3248,13 @@
         <v>107</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>71</v>
@@ -3268,7 +3263,7 @@
         <v>95</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>71</v>
@@ -3286,7 +3281,7 @@
         <v>101</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>82</v>
@@ -3294,8 +3289,8 @@
       <c r="T23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U23" s="17" t="s">
-        <v>129</v>
+      <c r="U23" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V23" s="1" t="s">
         <v>63</v>
@@ -3310,13 +3305,13 @@
         <v>102</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3328,7 +3323,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="1">
         <v>5782</v>
@@ -3341,16 +3336,16 @@
         <v>wild-type</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>72</v>
@@ -3359,7 +3354,7 @@
         <v>100</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>72</v>
@@ -3377,7 +3372,7 @@
         <v>105</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>83</v>
@@ -3385,8 +3380,8 @@
       <c r="T24" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U24" s="17" t="s">
-        <v>129</v>
+      <c r="U24" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>63</v>
@@ -3401,25 +3396,25 @@
         <v>102</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="2">
         <v>7081</v>
@@ -3435,13 +3430,13 @@
         <v>104</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>72</v>
@@ -3450,7 +3445,7 @@
         <v>100</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>72</v>
@@ -3468,7 +3463,7 @@
         <v>105</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>83</v>
@@ -3476,8 +3471,8 @@
       <c r="T25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U25" s="18" t="s">
-        <v>129</v>
+      <c r="U25" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>63</v>
@@ -3492,13 +3487,13 @@
         <v>102</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3510,7 +3505,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" s="1">
         <v>7078</v>
@@ -3526,13 +3521,13 @@
         <v>107</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>71</v>
@@ -3541,7 +3536,7 @@
         <v>95</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>71</v>
@@ -3559,7 +3554,7 @@
         <v>105</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S26" s="1" t="s">
         <v>83</v>
@@ -3567,8 +3562,8 @@
       <c r="T26" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U26" s="17" t="s">
-        <v>129</v>
+      <c r="U26" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>63</v>
@@ -3583,13 +3578,13 @@
         <v>102</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3601,7 +3596,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="1">
         <v>5782</v>
@@ -3614,16 +3609,16 @@
         <v>wild-type</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>72</v>
@@ -3632,7 +3627,7 @@
         <v>100</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>72</v>
@@ -3650,7 +3645,7 @@
         <v>105</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>83</v>
@@ -3658,8 +3653,8 @@
       <c r="T27" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U27" s="17" t="s">
-        <v>129</v>
+      <c r="U27" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>63</v>
@@ -3674,25 +3669,25 @@
         <v>102</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="2">
         <v>7081</v>
@@ -3708,13 +3703,13 @@
         <v>104</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>72</v>
@@ -3723,7 +3718,7 @@
         <v>100</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>72</v>
@@ -3741,7 +3736,7 @@
         <v>105</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>83</v>
@@ -3749,8 +3744,8 @@
       <c r="T28" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U28" s="18" t="s">
-        <v>129</v>
+      <c r="U28" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V28" s="2" t="s">
         <v>63</v>
@@ -3765,13 +3760,13 @@
         <v>102</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3783,7 +3778,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" s="1">
         <v>7078</v>
@@ -3799,13 +3794,13 @@
         <v>107</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>71</v>
@@ -3814,7 +3809,7 @@
         <v>95</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>71</v>
@@ -3832,7 +3827,7 @@
         <v>105</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>83</v>
@@ -3840,8 +3835,8 @@
       <c r="T29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U29" s="17" t="s">
-        <v>129</v>
+      <c r="U29" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>63</v>
@@ -3856,13 +3851,13 @@
         <v>102</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3874,7 +3869,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="1">
         <v>5782</v>
@@ -3887,16 +3882,16 @@
         <v>wild-type</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>72</v>
@@ -3905,7 +3900,7 @@
         <v>100</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>72</v>
@@ -3923,7 +3918,7 @@
         <v>108</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>84</v>
@@ -3931,8 +3926,8 @@
       <c r="T30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U30" s="17" t="s">
-        <v>129</v>
+      <c r="U30" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>63</v>
@@ -3947,25 +3942,25 @@
         <v>102</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB30" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC30" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="2">
         <v>7081</v>
@@ -3981,13 +3976,13 @@
         <v>104</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>72</v>
@@ -3996,7 +3991,7 @@
         <v>100</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>72</v>
@@ -4014,7 +4009,7 @@
         <v>108</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>84</v>
@@ -4022,8 +4017,8 @@
       <c r="T31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="U31" s="18" t="s">
-        <v>129</v>
+      <c r="U31" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="V31" s="2" t="s">
         <v>63</v>
@@ -4038,13 +4033,13 @@
         <v>102</v>
       </c>
       <c r="Z31" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC31" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4052,90 +4047,90 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="17">
+      <c r="B32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="1">
         <v>7078</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="17" t="str">
+      <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>rrp6-null</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" s="17" t="s">
+      <c r="G32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J32" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="K32" s="1" t="s">
         <v>95</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="M32" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O32" s="17" t="s">
+      <c r="O32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="17" t="s">
+      <c r="P32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" s="17" t="s">
+      <c r="Q32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R32" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="S32" s="17" t="s">
+      <c r="R32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S32" s="1" t="s">
         <v>84</v>
       </c>
       <c r="T32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U32" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="V32" s="17" t="s">
+      <c r="U32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V32" s="1" t="s">
         <v>63</v>
       </c>
       <c r="W32" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="X32" s="17" t="s">
+      <c r="X32" s="1" t="s">
         <v>88</v>
       </c>
       <c r="Y32" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="Z32" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA32" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB32" s="17" t="s">
-        <v>218</v>
+      <c r="Z32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="AC32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4147,7 +4142,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="1">
         <v>7718</v>
@@ -4162,13 +4157,13 @@
         <v>111</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>100</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>72</v>
@@ -4177,7 +4172,7 @@
         <v>100</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>72</v>
@@ -4195,7 +4190,7 @@
         <v>99</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>81</v>
@@ -4203,8 +4198,8 @@
       <c r="T33" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U33" s="17" t="s">
-        <v>130</v>
+      <c r="U33" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V33" s="4" t="s">
         <v>64</v>
@@ -4219,13 +4214,13 @@
         <v>98</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB33" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4237,7 +4232,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" s="1">
         <v>7718</v>
@@ -4252,13 +4247,13 @@
         <v>111</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>100</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>72</v>
@@ -4267,7 +4262,7 @@
         <v>100</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>72</v>
@@ -4285,7 +4280,7 @@
         <v>99</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>81</v>
@@ -4293,8 +4288,8 @@
       <c r="T34" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U34" s="17" t="s">
-        <v>130</v>
+      <c r="U34" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>63</v>
@@ -4309,13 +4304,13 @@
         <v>98</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB34" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4327,29 +4322,29 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="1">
         <v>6125</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="E35" s="1" t="str">
         <f>D35</f>
-        <v>Ostir-depletion</v>
+        <v>OsTIR-depletion</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>71</v>
@@ -4358,7 +4353,7 @@
         <v>95</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>71</v>
@@ -4376,7 +4371,7 @@
         <v>99</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S35" s="1" t="s">
         <v>81</v>
@@ -4384,8 +4379,8 @@
       <c r="T35" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U35" s="17" t="s">
-        <v>130</v>
+      <c r="U35" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V35" s="4" t="s">
         <v>64</v>
@@ -4400,13 +4395,13 @@
         <v>98</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB35" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4418,29 +4413,29 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="1">
         <v>6125</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>D36</f>
-        <v>Ostir-depletion</v>
+        <v>OsTIR-depletion</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>71</v>
@@ -4449,7 +4444,7 @@
         <v>95</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>71</v>
@@ -4467,7 +4462,7 @@
         <v>99</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S36" s="1" t="s">
         <v>81</v>
@@ -4475,8 +4470,8 @@
       <c r="T36" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U36" s="17" t="s">
-        <v>130</v>
+      <c r="U36" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V36" s="1" t="s">
         <v>63</v>
@@ -4491,13 +4486,13 @@
         <v>98</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB36" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4509,29 +4504,29 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C37" s="1">
         <v>6126</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="E37" s="1" t="str">
         <f>D37</f>
-        <v>Ostir-depletion</v>
+        <v>OsTIR-depletion</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>72</v>
@@ -4540,7 +4535,7 @@
         <v>100</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>72</v>
@@ -4558,7 +4553,7 @@
         <v>99</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>81</v>
@@ -4566,8 +4561,8 @@
       <c r="T37" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U37" s="17" t="s">
-        <v>130</v>
+      <c r="U37" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V37" s="4" t="s">
         <v>64</v>
@@ -4582,13 +4577,13 @@
         <v>98</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA37" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB37" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4600,29 +4595,29 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="1">
         <v>6126</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="E38" s="1" t="str">
         <f>D38</f>
-        <v>Ostir-depletion</v>
+        <v>OsTIR-depletion</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>72</v>
@@ -4631,7 +4626,7 @@
         <v>100</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>72</v>
@@ -4649,7 +4644,7 @@
         <v>99</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>81</v>
@@ -4657,8 +4652,8 @@
       <c r="T38" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="U38" s="17" t="s">
-        <v>130</v>
+      <c r="U38" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>63</v>
@@ -4673,13 +4668,13 @@
         <v>98</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB38" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC38" s="1" t="str">
         <f>_xlfn.CONCAT(F38, "_", N38, "_", R38, "_", AB38, "_", W38, "_",  T38, "_", Y38, "_", I38)</f>
@@ -4691,13 +4686,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="3">
         <v>7714</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>110</v>
@@ -4706,22 +4701,22 @@
         <v>111</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>95</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>73</v>
@@ -4739,7 +4734,7 @@
         <v>99</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S39" s="3" t="s">
         <v>81</v>
@@ -4747,8 +4742,8 @@
       <c r="T39" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="U39" s="19" t="s">
-        <v>130</v>
+      <c r="U39" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="V39" s="3" t="s">
         <v>64</v>
@@ -4763,32 +4758,32 @@
         <v>98</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB39" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC39" s="3" t="str">
         <f>_xlfn.CONCAT(F39, "_", N39, "_", R39, "_", AB39, "_", W39, "_", T39, "_", Y39, "_", L39)</f>
         <v>n3-d_Q_day7_tcn_N_aux-T_tc-F_rep3</v>
       </c>
-      <c r="AD39" s="19"/>
+      <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C40" s="3">
         <v>7714</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>110</v>
@@ -4797,22 +4792,22 @@
         <v>111</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>95</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>73</v>
@@ -4830,7 +4825,7 @@
         <v>99</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S40" s="3" t="s">
         <v>81</v>
@@ -4838,8 +4833,8 @@
       <c r="T40" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="U40" s="19" t="s">
-        <v>130</v>
+      <c r="U40" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="V40" s="3" t="s">
         <v>63</v>
@@ -4854,13 +4849,13 @@
         <v>98</v>
       </c>
       <c r="Z40" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB40" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC40" s="3" t="str">
         <f t="shared" ref="AC40:AC42" si="2">_xlfn.CONCAT(F40, "_", N40, "_", R40, "_", AB40, "_", W40, "_", T40, "_", Y40, "_", L40)</f>
@@ -4872,7 +4867,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C41" s="3">
         <v>7716</v>
@@ -4887,13 +4882,13 @@
         <v>111</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>95</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>71</v>
@@ -4902,7 +4897,7 @@
         <v>95</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>71</v>
@@ -4920,7 +4915,7 @@
         <v>99</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S41" s="3" t="s">
         <v>81</v>
@@ -4928,8 +4923,8 @@
       <c r="T41" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="U41" s="19" t="s">
-        <v>130</v>
+      <c r="U41" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="V41" s="3" t="s">
         <v>64</v>
@@ -4944,13 +4939,13 @@
         <v>98</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA41" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB41" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC41" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4962,7 +4957,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" s="3">
         <v>7716</v>
@@ -4977,13 +4972,13 @@
         <v>111</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>95</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>71</v>
@@ -4992,7 +4987,7 @@
         <v>95</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>71</v>
@@ -5010,7 +5005,7 @@
         <v>99</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S42" s="3" t="s">
         <v>81</v>
@@ -5018,8 +5013,8 @@
       <c r="T42" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="U42" s="19" t="s">
-        <v>130</v>
+      <c r="U42" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="V42" s="3" t="s">
         <v>63</v>
@@ -5034,13 +5029,13 @@
         <v>98</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA42" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB42" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC42" s="3" t="str">
         <f t="shared" si="2"/>
@@ -5052,7 +5047,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C43" s="1">
         <v>5782</v>
@@ -5065,25 +5060,25 @@
         <v>wild-type</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>72</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>73</v>
@@ -5101,7 +5096,7 @@
         <v>99</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S43" s="1" t="s">
         <v>81</v>
@@ -5109,8 +5104,8 @@
       <c r="T43" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U43" s="17" t="s">
-        <v>129</v>
+      <c r="U43" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V43" s="4" t="s">
         <v>64</v>
@@ -5125,13 +5120,13 @@
         <v>98</v>
       </c>
       <c r="Z43" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA43" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB43" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC43" s="1" t="str">
         <f t="shared" ref="AC43:AC56" si="4">_xlfn.CONCAT(F43, "_", N43, "_", R43, "_", AB43, "_", W43, "_",  T43, "_", Y43, "_", I43)</f>
@@ -5143,7 +5138,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C44" s="1">
         <v>5782</v>
@@ -5156,25 +5151,25 @@
         <v>wild-type</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>72</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>73</v>
@@ -5192,7 +5187,7 @@
         <v>99</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S44" s="1" t="s">
         <v>81</v>
@@ -5200,8 +5195,8 @@
       <c r="T44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U44" s="17" t="s">
-        <v>129</v>
+      <c r="U44" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>63</v>
@@ -5216,13 +5211,13 @@
         <v>98</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB44" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC44" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5234,29 +5229,29 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C45" s="1">
         <v>7747</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>71</v>
@@ -5265,7 +5260,7 @@
         <v>95</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>71</v>
@@ -5280,10 +5275,10 @@
         <v>59</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S45" s="1" t="s">
         <v>85</v>
@@ -5291,8 +5286,8 @@
       <c r="T45" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U45" s="17" t="s">
-        <v>129</v>
+      <c r="U45" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V45" s="1" t="s">
         <v>63</v>
@@ -5307,13 +5302,13 @@
         <v>98</v>
       </c>
       <c r="Z45" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA45" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB45" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC45" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5325,29 +5320,29 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C46" s="1">
         <v>7747</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>71</v>
@@ -5356,7 +5351,7 @@
         <v>95</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>71</v>
@@ -5371,10 +5366,10 @@
         <v>59</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S46" s="1" t="s">
         <v>85</v>
@@ -5382,8 +5377,8 @@
       <c r="T46" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U46" s="17" t="s">
-        <v>129</v>
+      <c r="U46" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V46" s="4" t="s">
         <v>64</v>
@@ -5398,13 +5393,13 @@
         <v>98</v>
       </c>
       <c r="Z46" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB46" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC46" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5416,29 +5411,29 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C47" s="1">
         <v>7748</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>72</v>
@@ -5447,7 +5442,7 @@
         <v>100</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>72</v>
@@ -5462,10 +5457,10 @@
         <v>59</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S47" s="1" t="s">
         <v>85</v>
@@ -5473,8 +5468,8 @@
       <c r="T47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U47" s="17" t="s">
-        <v>129</v>
+      <c r="U47" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>63</v>
@@ -5489,13 +5484,13 @@
         <v>98</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA47" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB47" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC47" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5507,29 +5502,29 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C48" s="1">
         <v>7748</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>72</v>
@@ -5538,7 +5533,7 @@
         <v>100</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>72</v>
@@ -5553,10 +5548,10 @@
         <v>59</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>85</v>
@@ -5564,8 +5559,8 @@
       <c r="T48" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U48" s="17" t="s">
-        <v>129</v>
+      <c r="U48" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V48" s="4" t="s">
         <v>64</v>
@@ -5580,13 +5575,13 @@
         <v>98</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA48" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB48" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC48" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5598,7 +5593,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C49" s="1">
         <v>5781</v>
@@ -5611,29 +5606,29 @@
         <v>wild-type</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>71</v>
       </c>
       <c r="K49" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="L49" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="L49" s="10" t="s">
+      <c r="M49" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="M49" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="N49" s="5" t="s">
         <v>59</v>
       </c>
@@ -5644,10 +5639,10 @@
         <v>59</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S49" s="1" t="s">
         <v>85</v>
@@ -5655,8 +5650,8 @@
       <c r="T49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U49" s="17" t="s">
-        <v>129</v>
+      <c r="U49" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V49" s="1" t="s">
         <v>63</v>
@@ -5671,13 +5666,13 @@
         <v>98</v>
       </c>
       <c r="Z49" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB49" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC49" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5689,7 +5684,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C50" s="1">
         <v>5781</v>
@@ -5702,29 +5697,29 @@
         <v>wild-type</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>71</v>
       </c>
       <c r="K50" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="L50" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="L50" s="10" t="s">
+      <c r="M50" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="M50" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="N50" s="5" t="s">
         <v>59</v>
       </c>
@@ -5735,10 +5730,10 @@
         <v>59</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S50" s="1" t="s">
         <v>85</v>
@@ -5746,8 +5741,8 @@
       <c r="T50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U50" s="17" t="s">
-        <v>129</v>
+      <c r="U50" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V50" s="4" t="s">
         <v>64</v>
@@ -5762,13 +5757,13 @@
         <v>98</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA50" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC50" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5780,7 +5775,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C51" s="1">
         <v>5782</v>
@@ -5793,29 +5788,29 @@
         <v>wild-type</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>72</v>
       </c>
       <c r="K51" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="L51" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="L51" s="10" t="s">
+      <c r="M51" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="M51" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="N51" s="5" t="s">
         <v>59</v>
       </c>
@@ -5826,10 +5821,10 @@
         <v>59</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S51" s="1" t="s">
         <v>85</v>
@@ -5837,8 +5832,8 @@
       <c r="T51" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U51" s="17" t="s">
-        <v>129</v>
+      <c r="U51" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>63</v>
@@ -5853,13 +5848,13 @@
         <v>98</v>
       </c>
       <c r="Z51" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA51" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB51" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC51" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5871,7 +5866,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C52" s="1">
         <v>5782</v>
@@ -5884,29 +5879,29 @@
         <v>wild-type</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>72</v>
       </c>
       <c r="K52" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="L52" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="L52" s="10" t="s">
+      <c r="M52" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="M52" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="N52" s="5" t="s">
         <v>59</v>
       </c>
@@ -5917,10 +5912,10 @@
         <v>59</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S52" s="1" t="s">
         <v>85</v>
@@ -5928,8 +5923,8 @@
       <c r="T52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U52" s="17" t="s">
-        <v>129</v>
+      <c r="U52" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V52" s="4" t="s">
         <v>64</v>
@@ -5944,13 +5939,13 @@
         <v>98</v>
       </c>
       <c r="Z52" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA52" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB52" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC52" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5962,7 +5957,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C53" s="1">
         <v>7078</v>
@@ -5978,13 +5973,13 @@
         <v>107</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>71</v>
@@ -5993,7 +5988,7 @@
         <v>95</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>71</v>
@@ -6008,10 +6003,10 @@
         <v>59</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>85</v>
@@ -6019,8 +6014,8 @@
       <c r="T53" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U53" s="17" t="s">
-        <v>129</v>
+      <c r="U53" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V53" s="1" t="s">
         <v>63</v>
@@ -6035,13 +6030,13 @@
         <v>98</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA53" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB53" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC53" s="1" t="str">
         <f t="shared" si="4"/>
@@ -6053,7 +6048,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C54" s="1">
         <v>7078</v>
@@ -6069,13 +6064,13 @@
         <v>107</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>71</v>
@@ -6084,7 +6079,7 @@
         <v>95</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>71</v>
@@ -6099,10 +6094,10 @@
         <v>59</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S54" s="1" t="s">
         <v>85</v>
@@ -6110,8 +6105,8 @@
       <c r="T54" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U54" s="17" t="s">
-        <v>129</v>
+      <c r="U54" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V54" s="4" t="s">
         <v>64</v>
@@ -6126,13 +6121,13 @@
         <v>98</v>
       </c>
       <c r="Z54" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA54" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB54" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC54" s="1" t="str">
         <f t="shared" si="4"/>
@@ -6144,7 +6139,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C55" s="1">
         <v>7079</v>
@@ -6160,13 +6155,13 @@
         <v>107</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>72</v>
@@ -6175,7 +6170,7 @@
         <v>100</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>72</v>
@@ -6190,10 +6185,10 @@
         <v>59</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S55" s="1" t="s">
         <v>85</v>
@@ -6201,8 +6196,8 @@
       <c r="T55" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U55" s="17" t="s">
-        <v>129</v>
+      <c r="U55" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V55" s="1" t="s">
         <v>63</v>
@@ -6217,13 +6212,13 @@
         <v>98</v>
       </c>
       <c r="Z55" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA55" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB55" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC55" s="1" t="str">
         <f t="shared" si="4"/>
@@ -6235,7 +6230,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C56" s="1">
         <v>7079</v>
@@ -6251,13 +6246,13 @@
         <v>107</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>72</v>
@@ -6266,7 +6261,7 @@
         <v>100</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>72</v>
@@ -6281,10 +6276,10 @@
         <v>59</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S56" s="1" t="s">
         <v>85</v>
@@ -6292,8 +6287,8 @@
       <c r="T56" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U56" s="17" t="s">
-        <v>129</v>
+      <c r="U56" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="V56" s="4" t="s">
         <v>64</v>
@@ -6308,13 +6303,13 @@
         <v>98</v>
       </c>
       <c r="Z56" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB56" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC56" s="1" t="str">
         <f t="shared" si="4"/>
@@ -6341,93 +6336,93 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" t="s">
         <v>203</v>
       </c>
-      <c r="B1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" t="s">
-        <v>204</v>
-      </c>
       <c r="D1" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
See notes for 2023-0421; pushed files include snRNA/snoRNA work, corrected batch-labeling errors in variables.xlsx, and began work for the counts per feature categeory panel in Figure 1 (see work_assess_R64-1-1_gff3.Rmd (to be renamed))
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22BF203-DC32-F74E-805E-DDFFD84BFD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE8AFE-540B-014E-9200-B433C90FDB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="500" windowWidth="37480" windowHeight="28300" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="3660" yWindow="500" windowWidth="47540" windowHeight="28300" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
-    <sheet name="fix work_count_features.md" sheetId="3" r:id="rId2"/>
+    <sheet name="correct-batch-labels" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="261">
   <si>
     <t>5781_G1_IN</t>
   </si>
@@ -612,27 +612,6 @@
     <t>r4</t>
   </si>
   <si>
-    <t>r6-n_DSm2_day2_SS_rep1</t>
-  </si>
-  <si>
-    <t>r6-n_DSp2_day2_SS_rep1</t>
-  </si>
-  <si>
-    <t>r6-n_DSp24_day3_SS_rep1</t>
-  </si>
-  <si>
-    <t>r6-n_DSp48_day4_SS_rep2</t>
-  </si>
-  <si>
-    <t>r6-n_DSm2_day2_SS_rep2</t>
-  </si>
-  <si>
-    <t>r6-n_DSp2_day2_SS_rep2</t>
-  </si>
-  <si>
-    <t>r6-n_DSp24_day3_SS_rep2</t>
-  </si>
-  <si>
     <t>rep-5</t>
   </si>
   <si>
@@ -642,79 +621,6 @@
     <t>r5</t>
   </si>
   <si>
-    <t>r6-n_DSp48_day4_SS_rep1</t>
-  </si>
-  <si>
-    <t>incorrect</t>
-  </si>
-  <si>
-    <t>correct</t>
-  </si>
-  <si>
-    <t>intermediate</t>
-  </si>
-  <si>
-    <t>r6-n_DSm2_day2_SS_x-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSp2_day2_SS_x-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSp24_day3_SS_x-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSm2_day2_SS_y-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSp2_day2_SS_y-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSp24_day3_SS_y-dekho</t>
-  </si>
-  <si>
-    <t>r6-n_DSp48_day4_SS_y-dekho</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="2"/>
-      </rPr>
-      <t>#TODO</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> replace x-dekho with rep2; replace y-dekho with rep1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Done.</t>
-    </r>
-  </si>
-  <si>
     <t>kit</t>
   </si>
   <si>
@@ -794,13 +700,133 @@
   </si>
   <si>
     <t>tech2</t>
+  </si>
+  <si>
+    <t>BM10_5781_DSp48_S26_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM10_5781_DSp48_S26_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM10_5781_DSp48_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM10_5781_DSp48_S26_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM10_5781_DSp48_S26_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM12_7079_DSp48_S27_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM12_7079_DSp48_S27_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM12_7079_DSp48_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM12_7079_DSp48_S27_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BM12_7079_DSp48_S27_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>CW6_7078_day8_Q_SS_S28_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>CW6_7078_day8_Q_SS_S28_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>CW6_7078_day8_Q_SS_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>CW6_7078_day8_Q_SS_S28_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>CW6_7078_day8_Q_SS_S28_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA1_5781_SS_G1_S22_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA1_5781_SS_G1_S22_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA1_5781_SS_G1_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA1_5781_SS_G1_S22_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA1_5781_SS_G1_S22_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA2_5782_SS_G1_S23_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA2_5782_SS_G1_S23_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA2_5782_SS_G1_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA2_5782_SS_G1_S23_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA2_5782_SS_G1_S23_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA3_7078_SS_G1_S24_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA3_7078_SS_G1_S24_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA3_7078_SS_G1_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA3_7078_SS_G1_S24_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA3_7078_SS_G1_S24_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA4_7079_SS_G1_S25_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA4_7079_SS_G1_S25_I2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA4_7079_SS_G1_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA4_7079_SS_G1_S25_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>DA4_7079_SS_G1_S25_R3_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</t>
+  </si>
+  <si>
+    <t>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1_tech2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2_tech1</t>
+  </si>
+  <si>
+    <t>2023-0421: updated from tech1 to tech2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -860,39 +886,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,6 +911,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -924,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -938,14 +944,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,10 +1368,10 @@
         <v>186</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>57</v>
@@ -1405,19 +1413,19 @@
         <v>132</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -1462,10 +1470,10 @@
         <v>71</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>58</v>
@@ -1507,17 +1515,17 @@
         <v>130</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE2" s="1" t="str">
         <f>_xlfn.CONCAT(F2, "_", P2, "_", T2, "_", AD2, "_", Y2, "_",  V2, "_", AA2, "_", I2)</f>
         <v>WT_G1_day1_ovn_SS_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF2" s="1" t="str">
-        <f>_xlfn.CONCAT(F2, "_", P2, "_", T2, "_", AD2, "_", Y2, "_",  V2, "_", AA2, "_", I2, "_", O2)</f>
+        <f t="shared" ref="AF2:AF40" si="1">_xlfn.CONCAT(F2, "_", P2, "_", T2, "_", AD2, "_", Y2, "_",  V2, "_", AA2, "_", I2, "_", O2)</f>
         <v>WT_G1_day1_ovn_SS_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG2" t="b">
@@ -1566,10 +1574,10 @@
         <v>71</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>58</v>
@@ -1611,17 +1619,17 @@
         <v>130</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE3" s="1" t="str">
-        <f t="shared" ref="AE3:AE39" si="1">_xlfn.CONCAT(F3, "_", P3, "_", T3, "_", AD3, "_", Y3, "_",  V3, "_", AA3, "_", I3)</f>
+        <f t="shared" ref="AE3:AE39" si="2">_xlfn.CONCAT(F3, "_", P3, "_", T3, "_", AD3, "_", Y3, "_",  V3, "_", AA3, "_", I3)</f>
         <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF3" s="1" t="str">
-        <f>_xlfn.CONCAT(F3, "_", P3, "_", T3, "_", AD3, "_", Y3, "_",  V3, "_", AA3, "_", I3, "_", O3)</f>
+        <f t="shared" si="1"/>
         <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG3" t="b">
@@ -1670,10 +1678,10 @@
         <v>71</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>59</v>
@@ -1715,17 +1723,17 @@
         <v>130</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep1</v>
+      </c>
+      <c r="AF4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep1</v>
-      </c>
-      <c r="AF4" s="1" t="str">
-        <f>_xlfn.CONCAT(F4, "_", P4, "_", T4, "_", AD4, "_", Y4, "_",  V4, "_", AA4, "_", I4, "_", O4)</f>
         <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG4" t="b">
@@ -1774,10 +1782,10 @@
         <v>71</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>59</v>
@@ -1819,17 +1827,17 @@
         <v>130</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep1</v>
+      </c>
+      <c r="AF5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep1</v>
-      </c>
-      <c r="AF5" s="1" t="str">
-        <f>_xlfn.CONCAT(F5, "_", P5, "_", T5, "_", AD5, "_", Y5, "_",  V5, "_", AA5, "_", I5, "_", O5)</f>
         <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG5" t="b">
@@ -1878,10 +1886,10 @@
         <v>72</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>58</v>
@@ -1923,17 +1931,17 @@
         <v>130</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_G1_day1_ovn_SS_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AF6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_G1_day1_ovn_SS_aux-F_tc-F_rep2</v>
-      </c>
-      <c r="AF6" s="1" t="str">
-        <f>_xlfn.CONCAT(F6, "_", P6, "_", T6, "_", AD6, "_", Y6, "_",  V6, "_", AA6, "_", I6, "_", O6)</f>
         <v>WT_G1_day1_ovn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG6" t="b">
@@ -1982,10 +1990,10 @@
         <v>72</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>58</v>
@@ -2027,17 +2035,17 @@
         <v>130</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AF7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep2</v>
-      </c>
-      <c r="AF7" s="1" t="str">
-        <f>_xlfn.CONCAT(F7, "_", P7, "_", T7, "_", AD7, "_", Y7, "_",  V7, "_", AA7, "_", I7, "_", O7)</f>
         <v>WT_G1_day1_ovn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG7" t="b">
@@ -2086,10 +2094,10 @@
         <v>72</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>59</v>
@@ -2131,17 +2139,17 @@
         <v>130</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AF8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep2</v>
-      </c>
-      <c r="AF8" s="1" t="str">
-        <f>_xlfn.CONCAT(F8, "_", P8, "_", T8, "_", AD8, "_", Y8, "_",  V8, "_", AA8, "_", I8, "_", O8)</f>
         <v>WT_Q_day7_ovn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG8" t="b">
@@ -2190,10 +2198,10 @@
         <v>72</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>59</v>
@@ -2235,17 +2243,17 @@
         <v>130</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AE9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AF9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep2</v>
-      </c>
-      <c r="AF9" s="1" t="str">
-        <f>_xlfn.CONCAT(F9, "_", P9, "_", T9, "_", AD9, "_", Y9, "_",  V9, "_", AA9, "_", I9, "_", O9)</f>
         <v>WT_Q_day7_ovn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG9" t="b">
@@ -2253,103 +2261,103 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>5781</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="16" t="str">
+      <c r="E10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>wild-type</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="N10" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="Q10" s="16" t="s">
+      <c r="Q10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="R10" s="16" t="s">
+      <c r="R10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="S10" s="16" t="s">
+      <c r="S10" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="16" t="s">
+      <c r="T10" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="V10" s="17" t="s">
+      <c r="V10" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="W10" s="16" t="s">
+      <c r="W10" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="X10" s="16" t="s">
+      <c r="X10" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y10" s="17" t="s">
+      <c r="Y10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z10" s="16" t="s">
+      <c r="Z10" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA10" s="17" t="s">
+      <c r="AA10" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AB10" s="16" t="s">
+      <c r="AB10" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="AC10" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD10" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE10" s="16" t="str">
+      <c r="AC10" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD10" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE10" s="15" t="str">
         <f>_xlfn.CONCAT(F10, "_", P10, "_", T10, "_", AD10, "_", Y10, "_",  V10, "_", AA10, "_", I10)</f>
         <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
       </c>
-      <c r="AF10" s="16" t="str">
-        <f>_xlfn.CONCAT(F10, "_", P10, "_", T10, "_", AD10, "_", Y10, "_",  V10, "_", AA10, "_", I10, "_", O10)</f>
+      <c r="AF10" s="15" t="str">
+        <f t="shared" si="1"/>
         <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG10" s="12" t="b">
@@ -2357,109 +2365,107 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>5781</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="N11" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="R11" s="16" t="s">
+      <c r="R11" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="S11" s="16" t="s">
+      <c r="S11" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="T11" s="16" t="s">
+      <c r="T11" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="V11" s="18" t="s">
+      <c r="V11" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="W11" s="16" t="s">
+      <c r="W11" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="X11" s="16" t="s">
+      <c r="X11" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y11" s="17" t="s">
+      <c r="Y11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z11" s="16" t="s">
+      <c r="Z11" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA11" s="17" t="s">
+      <c r="AA11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AB11" s="16" t="s">
+      <c r="AB11" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="AC11" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD11" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE11" s="16" t="str">
-        <f>_xlfn.CONCAT(F11, "_", P11, "_", T11, "_", AD11, "_", Y11, "_",  V11, "_", AA11, "_", I11)</f>
-        <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF11" s="16" t="str">
-        <f>_xlfn.CONCAT(F11, "_", P11, "_", T11, "_", AD11, "_", Y11, "_",  V11, "_", AA11, "_", I11, "_", O11)</f>
-        <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep1_tech2</v>
-      </c>
-      <c r="AG11" s="20" t="b">
+      <c r="AC11" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD11" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE11" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF11" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="AG11" s="19" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2501,10 +2507,10 @@
         <v>71</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>66</v>
@@ -2546,29 +2552,29 @@
         <v>131</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF12" s="2" t="str">
-        <f>_xlfn.CONCAT(F12, "_", P12, "_", T12, "_", AD12, "_", Y12, "_",  V12, "_", AA12, "_", I12, "_", O12)</f>
         <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
-      <c r="AG12" s="14" t="b">
+      <c r="AG12" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C13" s="1">
         <v>7079</v>
@@ -2603,11 +2609,11 @@
       <c r="M13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>238</v>
+      <c r="N13" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>66</v>
@@ -2627,7 +2633,7 @@
       <c r="U13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="V13" s="15" t="s">
+      <c r="V13" s="14" t="s">
         <v>97</v>
       </c>
       <c r="W13" s="1" t="s">
@@ -2649,24 +2655,22 @@
         <v>131</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE13" s="1" t="str">
-        <f>_xlfn.CONCAT(F13, "_", P13, "_", T13, "_", AD13, "_", Y13, "_",  V13, "_", AA13, "_", I13)</f>
-        <v>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF13" s="1" t="str">
-        <f>_xlfn.CONCAT(F13, "_", P13, "_", T13, "_", AD13, "_", Y13, "_",  V13, "_", AA13, "_", I13, "_", O13)</f>
-        <v>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2_tech1</v>
-      </c>
-      <c r="AG13" s="19" t="b">
+        <v>198</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AG13" s="18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2708,10 +2712,10 @@
         <v>71</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>67</v>
@@ -2753,17 +2757,17 @@
         <v>131</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF14" s="1" t="str">
-        <f>_xlfn.CONCAT(F14, "_", P14, "_", T14, "_", AD14, "_", Y14, "_",  V14, "_", AA14, "_", I14, "_", O14)</f>
         <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG14" t="b">
@@ -2812,10 +2816,10 @@
         <v>71</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>67</v>
@@ -2857,20 +2861,20 @@
         <v>131</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF15" s="2" t="str">
-        <f>_xlfn.CONCAT(F15, "_", P15, "_", T15, "_", AD15, "_", Y15, "_",  V15, "_", AA15, "_", I15, "_", O15)</f>
         <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
-      <c r="AG15" s="14" t="b">
+      <c r="AG15" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2916,10 +2920,10 @@
         <v>72</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>67</v>
@@ -2961,24 +2965,24 @@
         <v>131</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF16" s="1" t="str">
-        <f>_xlfn.CONCAT(F16, "_", P16, "_", T16, "_", AD16, "_", Y16, "_",  V16, "_", AA16, "_", I16, "_", O16)</f>
         <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3020,10 +3024,10 @@
         <v>71</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>68</v>
@@ -3065,17 +3069,17 @@
         <v>131</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF17" s="1" t="str">
-        <f>_xlfn.CONCAT(F17, "_", P17, "_", T17, "_", AD17, "_", Y17, "_",  V17, "_", AA17, "_", I17, "_", O17)</f>
         <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG17" t="b">
@@ -3124,10 +3128,10 @@
         <v>71</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>68</v>
@@ -3169,20 +3173,20 @@
         <v>131</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF18" s="2" t="str">
-        <f>_xlfn.CONCAT(F18, "_", P18, "_", T18, "_", AD18, "_", Y18, "_",  V18, "_", AA18, "_", I18, "_", O18)</f>
         <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
-      <c r="AG18" s="14" t="b">
+      <c r="AG18" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3228,10 +3232,10 @@
         <v>72</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>68</v>
@@ -3273,24 +3277,24 @@
         <v>131</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF19" s="1" t="str">
-        <f>_xlfn.CONCAT(F19, "_", P19, "_", T19, "_", AD19, "_", Y19, "_",  V19, "_", AA19, "_", I19, "_", O19)</f>
         <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -3332,10 +3336,10 @@
         <v>71</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>69</v>
@@ -3377,17 +3381,17 @@
         <v>131</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF20" s="1" t="str">
-        <f>_xlfn.CONCAT(F20, "_", P20, "_", T20, "_", AD20, "_", Y20, "_",  V20, "_", AA20, "_", I20, "_", O20)</f>
         <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG20" t="b">
@@ -3436,10 +3440,10 @@
         <v>71</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>69</v>
@@ -3481,20 +3485,20 @@
         <v>131</v>
       </c>
       <c r="AC21" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF21" s="2" t="str">
-        <f>_xlfn.CONCAT(F21, "_", P21, "_", T21, "_", AD21, "_", Y21, "_",  V21, "_", AA21, "_", I21, "_", O21)</f>
         <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
-      <c r="AG21" s="14" t="b">
+      <c r="AG21" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3540,10 +3544,10 @@
         <v>72</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>69</v>
@@ -3585,24 +3589,24 @@
         <v>131</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF22" s="1" t="str">
-        <f>_xlfn.CONCAT(F22, "_", P22, "_", T22, "_", AD22, "_", Y22, "_",  V22, "_", AA22, "_", I22, "_", O22)</f>
         <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -3644,10 +3648,10 @@
         <v>72</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>66</v>
@@ -3689,17 +3693,17 @@
         <v>131</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD23" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF23" s="1" t="str">
-        <f>_xlfn.CONCAT(F23, "_", P23, "_", T23, "_", AD23, "_", Y23, "_",  V23, "_", AA23, "_", I23, "_", O23)</f>
         <v>WT_DSp48_day4_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG23" t="b">
@@ -3748,10 +3752,10 @@
         <v>72</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>66</v>
@@ -3793,20 +3797,20 @@
         <v>131</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF24" s="2" t="str">
-        <f>_xlfn.CONCAT(F24, "_", P24, "_", T24, "_", AD24, "_", Y24, "_",  V24, "_", AA24, "_", I24, "_", O24)</f>
         <v>t4-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
-      <c r="AG24" s="14" t="b">
+      <c r="AG24" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3852,10 +3856,10 @@
         <v>71</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>66</v>
@@ -3897,24 +3901,24 @@
         <v>131</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF25" s="1" t="str">
-        <f>_xlfn.CONCAT(F25, "_", P25, "_", T25, "_", AD25, "_", Y25, "_",  V25, "_", AA25, "_", I25, "_", O25)</f>
         <v>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -3956,10 +3960,10 @@
         <v>72</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>67</v>
@@ -4001,17 +4005,17 @@
         <v>131</v>
       </c>
       <c r="AC26" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD26" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF26" s="1" t="str">
-        <f>_xlfn.CONCAT(F26, "_", P26, "_", T26, "_", AD26, "_", Y26, "_",  V26, "_", AA26, "_", I26, "_", O26)</f>
         <v>WT_DSm2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG26" t="b">
@@ -4060,10 +4064,10 @@
         <v>72</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>67</v>
@@ -4105,20 +4109,20 @@
         <v>131</v>
       </c>
       <c r="AC27" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF27" s="2" t="str">
-        <f>_xlfn.CONCAT(F27, "_", P27, "_", T27, "_", AD27, "_", Y27, "_",  V27, "_", AA27, "_", I27, "_", O27)</f>
         <v>t4-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
-      <c r="AG27" s="14" t="b">
+      <c r="AG27" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4164,10 +4168,10 @@
         <v>71</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>67</v>
@@ -4209,24 +4213,24 @@
         <v>131</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD28" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF28" s="1" t="str">
-        <f>_xlfn.CONCAT(F28, "_", P28, "_", T28, "_", AD28, "_", Y28, "_",  V28, "_", AA28, "_", I28, "_", O28)</f>
         <v>r6-n_DSm2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -4268,10 +4272,10 @@
         <v>72</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>68</v>
@@ -4313,17 +4317,17 @@
         <v>131</v>
       </c>
       <c r="AC29" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD29" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF29" s="1" t="str">
-        <f>_xlfn.CONCAT(F29, "_", P29, "_", T29, "_", AD29, "_", Y29, "_",  V29, "_", AA29, "_", I29, "_", O29)</f>
         <v>WT_DSp2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG29" t="b">
@@ -4372,10 +4376,10 @@
         <v>72</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>68</v>
@@ -4417,20 +4421,20 @@
         <v>131</v>
       </c>
       <c r="AC30" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF30" s="2" t="str">
-        <f>_xlfn.CONCAT(F30, "_", P30, "_", T30, "_", AD30, "_", Y30, "_",  V30, "_", AA30, "_", I30, "_", O30)</f>
         <v>t4-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
-      <c r="AG30" s="14" t="b">
+      <c r="AG30" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4476,10 +4480,10 @@
         <v>71</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>68</v>
@@ -4521,24 +4525,24 @@
         <v>131</v>
       </c>
       <c r="AC31" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD31" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF31" s="1" t="str">
-        <f>_xlfn.CONCAT(F31, "_", P31, "_", T31, "_", AD31, "_", Y31, "_",  V31, "_", AA31, "_", I31, "_", O31)</f>
         <v>r6-n_DSp2_day2_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -4580,10 +4584,10 @@
         <v>72</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>69</v>
@@ -4625,17 +4629,17 @@
         <v>131</v>
       </c>
       <c r="AC32" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD32" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF32" s="1" t="str">
-        <f>_xlfn.CONCAT(F32, "_", P32, "_", T32, "_", AD32, "_", Y32, "_",  V32, "_", AA32, "_", I32, "_", O32)</f>
         <v>WT_DSp24_day3_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
       <c r="AG32" t="b">
@@ -4684,10 +4688,10 @@
         <v>72</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>69</v>
@@ -4729,20 +4733,20 @@
         <v>131</v>
       </c>
       <c r="AC33" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD33" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
+      </c>
+      <c r="AF33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2</v>
-      </c>
-      <c r="AF33" s="2" t="str">
-        <f>_xlfn.CONCAT(F33, "_", P33, "_", T33, "_", AD33, "_", Y33, "_",  V33, "_", AA33, "_", I33, "_", O33)</f>
         <v>t4-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep2_tech1</v>
       </c>
-      <c r="AG33" s="14" t="b">
+      <c r="AG33" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4788,10 +4792,10 @@
         <v>71</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>69</v>
@@ -4833,17 +4837,17 @@
         <v>131</v>
       </c>
       <c r="AC34" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD34" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
+      </c>
+      <c r="AF34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1</v>
-      </c>
-      <c r="AF34" s="1" t="str">
-        <f>_xlfn.CONCAT(F34, "_", P34, "_", T34, "_", AD34, "_", Y34, "_",  V34, "_", AA34, "_", I34, "_", O34)</f>
         <v>r6-n_DSp24_day3_tcn_SS_aux-F_tc-T_rep1_tech1</v>
       </c>
       <c r="AG34" t="b">
@@ -4891,10 +4895,10 @@
         <v>72</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>59</v>
@@ -4936,17 +4940,17 @@
         <v>130</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD35" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>n3-d_Q_day7_tcn_N_aux-T_tc-F_rep2</v>
+      </c>
+      <c r="AF35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>n3-d_Q_day7_tcn_N_aux-T_tc-F_rep2</v>
-      </c>
-      <c r="AF35" s="1" t="str">
-        <f>_xlfn.CONCAT(F35, "_", P35, "_", T35, "_", AD35, "_", Y35, "_",  V35, "_", AA35, "_", I35, "_", O35)</f>
         <v>n3-d_Q_day7_tcn_N_aux-T_tc-F_rep2_tech1</v>
       </c>
       <c r="AG35" t="b">
@@ -4994,10 +4998,10 @@
         <v>72</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>59</v>
@@ -5039,17 +5043,17 @@
         <v>130</v>
       </c>
       <c r="AC36" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>n3-d_Q_day7_tcn_SS_aux-T_tc-F_rep2</v>
+      </c>
+      <c r="AF36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>n3-d_Q_day7_tcn_SS_aux-T_tc-F_rep2</v>
-      </c>
-      <c r="AF36" s="1" t="str">
-        <f>_xlfn.CONCAT(F36, "_", P36, "_", T36, "_", AD36, "_", Y36, "_",  V36, "_", AA36, "_", I36, "_", O36)</f>
         <v>n3-d_Q_day7_tcn_SS_aux-T_tc-F_rep2_tech1</v>
       </c>
       <c r="AG36" t="b">
@@ -5067,7 +5071,7 @@
         <v>6125</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="E37" s="1" t="str">
         <f>D37</f>
@@ -5098,10 +5102,10 @@
         <v>71</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>59</v>
@@ -5143,17 +5147,17 @@
         <v>130</v>
       </c>
       <c r="AC37" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep1</v>
+      </c>
+      <c r="AF37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep1</v>
-      </c>
-      <c r="AF37" s="1" t="str">
-        <f>_xlfn.CONCAT(F37, "_", P37, "_", T37, "_", AD37, "_", Y37, "_",  V37, "_", AA37, "_", I37, "_", O37)</f>
         <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep1_tech1</v>
       </c>
       <c r="AG37" t="b">
@@ -5171,7 +5175,7 @@
         <v>6125</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="str">
         <f>D38</f>
@@ -5202,10 +5206,10 @@
         <v>71</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>59</v>
@@ -5247,17 +5251,17 @@
         <v>130</v>
       </c>
       <c r="AC38" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>o-d_Q_day7_tcn_SS_aux-T_tc-F_rep1</v>
+      </c>
+      <c r="AF38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>o-d_Q_day7_tcn_SS_aux-T_tc-F_rep1</v>
-      </c>
-      <c r="AF38" s="1" t="str">
-        <f>_xlfn.CONCAT(F38, "_", P38, "_", T38, "_", AD38, "_", Y38, "_",  V38, "_", AA38, "_", I38, "_", O38)</f>
         <v>o-d_Q_day7_tcn_SS_aux-T_tc-F_rep1_tech1</v>
       </c>
       <c r="AG38" t="b">
@@ -5275,7 +5279,7 @@
         <v>6126</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="E39" s="1" t="str">
         <f>D39</f>
@@ -5306,10 +5310,10 @@
         <v>72</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>59</v>
@@ -5351,17 +5355,17 @@
         <v>130</v>
       </c>
       <c r="AC39" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep2</v>
+      </c>
+      <c r="AF39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep2</v>
-      </c>
-      <c r="AF39" s="1" t="str">
-        <f>_xlfn.CONCAT(F39, "_", P39, "_", T39, "_", AD39, "_", Y39, "_",  V39, "_", AA39, "_", I39, "_", O39)</f>
         <v>o-d_Q_day7_tcn_N_aux-T_tc-F_rep2_tech1</v>
       </c>
       <c r="AG39" t="b">
@@ -5379,7 +5383,7 @@
         <v>6126</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="E40" s="1" t="str">
         <f>D40</f>
@@ -5410,10 +5414,10 @@
         <v>72</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>59</v>
@@ -5455,17 +5459,17 @@
         <v>130</v>
       </c>
       <c r="AC40" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD40" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE40" s="1" t="str">
         <f>_xlfn.CONCAT(F40, "_", P40, "_", T40, "_", AD40, "_", Y40, "_",  V40, "_", AA40, "_", I40)</f>
         <v>o-d_Q_day7_tcn_SS_aux-T_tc-F_rep2</v>
       </c>
       <c r="AF40" s="1" t="str">
-        <f>_xlfn.CONCAT(F40, "_", P40, "_", T40, "_", AD40, "_", Y40, "_",  V40, "_", AA40, "_", I40, "_", O40)</f>
+        <f t="shared" si="1"/>
         <v>o-d_Q_day7_tcn_SS_aux-T_tc-F_rep2_tech1</v>
       </c>
       <c r="AG40" t="b">
@@ -5513,10 +5517,10 @@
         <v>73</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P41" s="7" t="s">
         <v>59</v>
@@ -5558,10 +5562,10 @@
         <v>130</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD41" s="3" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE41" s="3" t="str">
         <f>_xlfn.CONCAT(F41, "_", P41, "_", T41, "_", AD41, "_", Y41, "_", V41, "_", AA41, "_", L41)</f>
@@ -5616,10 +5620,10 @@
         <v>73</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P42" s="7" t="s">
         <v>59</v>
@@ -5661,10 +5665,10 @@
         <v>130</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD42" s="3" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE42" s="3" t="str">
         <f>_xlfn.CONCAT(F42, "_", P42, "_", T42, "_", AD42, "_", Y42, "_", V42, "_", AA42, "_", L42)</f>
@@ -5719,10 +5723,10 @@
         <v>71</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P43" s="7" t="s">
         <v>59</v>
@@ -5764,10 +5768,10 @@
         <v>130</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD43" s="3" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE43" s="3" t="str">
         <f>_xlfn.CONCAT(F43, "_", P43, "_", T43, "_", AD43, "_", Y43, "_", V43, "_", AA43, "_", L43)</f>
@@ -5822,10 +5826,10 @@
         <v>71</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P44" s="7" t="s">
         <v>59</v>
@@ -5867,10 +5871,10 @@
         <v>130</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD44" s="3" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE44" s="3" t="str">
         <f>_xlfn.CONCAT(F44, "_", P44, "_", T44, "_", AD44, "_", Y44, "_", V44, "_", AA44, "_", L44)</f>
@@ -5898,7 +5902,7 @@
         <v>56</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f t="shared" ref="E45:E59" si="2">D45</f>
+        <f t="shared" ref="E45:E59" si="3">D45</f>
         <v>wild-type</v>
       </c>
       <c r="F45" s="5" t="s">
@@ -5926,10 +5930,10 @@
         <v>73</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P45" s="5" t="s">
         <v>59</v>
@@ -5971,17 +5975,17 @@
         <v>130</v>
       </c>
       <c r="AC45" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD45" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE45" s="1" t="str">
-        <f t="shared" ref="AE45:AE63" si="3">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45)</f>
+        <f t="shared" ref="AE45:AE63" si="4">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45)</f>
         <v>WT_Q_day7_tcn_N_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF45" s="1" t="str">
-        <f>_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45, "_", O45)</f>
+        <f t="shared" ref="AF45:AF63" si="5">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45, "_", O45)</f>
         <v>WT_Q_day7_tcn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG45" t="b">
@@ -6002,7 +6006,7 @@
         <v>56</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wild-type</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -6030,10 +6034,10 @@
         <v>73</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>59</v>
@@ -6075,17 +6079,17 @@
         <v>130</v>
       </c>
       <c r="AC46" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD46" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE46" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WT_Q_day7_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF46" s="1" t="str">
-        <f>_xlfn.CONCAT(F46, "_", P46, "_", T46, "_", AD46, "_", Y46, "_",  V46, "_", AA46, "_", I46, "_", O46)</f>
+        <f t="shared" si="5"/>
         <v>WT_Q_day7_tcn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG46" t="b">
@@ -6106,7 +6110,7 @@
         <v>116</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F47" s="5" t="s">
@@ -6134,10 +6138,10 @@
         <v>71</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>59</v>
@@ -6179,17 +6183,17 @@
         <v>130</v>
       </c>
       <c r="AC47" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD47" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE47" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r1-n_Q_day8_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF47" s="1" t="str">
-        <f>_xlfn.CONCAT(F47, "_", P47, "_", T47, "_", AD47, "_", Y47, "_",  V47, "_", AA47, "_", I47, "_", O47)</f>
+        <f t="shared" si="5"/>
         <v>r1-n_Q_day8_tcn_SS_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG47" t="b">
@@ -6210,7 +6214,7 @@
         <v>116</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F48" s="5" t="s">
@@ -6238,10 +6242,10 @@
         <v>71</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>59</v>
@@ -6283,17 +6287,17 @@
         <v>130</v>
       </c>
       <c r="AC48" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE48" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r1-n_Q_day8_tcn_N_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF48" s="1" t="str">
-        <f>_xlfn.CONCAT(F48, "_", P48, "_", T48, "_", AD48, "_", Y48, "_",  V48, "_", AA48, "_", I48, "_", O48)</f>
+        <f t="shared" si="5"/>
         <v>r1-n_Q_day8_tcn_N_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG48" t="b">
@@ -6314,7 +6318,7 @@
         <v>116</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F49" s="5" t="s">
@@ -6342,10 +6346,10 @@
         <v>72</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>59</v>
@@ -6387,17 +6391,17 @@
         <v>130</v>
       </c>
       <c r="AC49" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD49" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE49" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r1-n_Q_day8_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF49" s="1" t="str">
-        <f>_xlfn.CONCAT(F49, "_", P49, "_", T49, "_", AD49, "_", Y49, "_",  V49, "_", AA49, "_", I49, "_", O49)</f>
+        <f t="shared" si="5"/>
         <v>r1-n_Q_day8_tcn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG49" t="b">
@@ -6418,7 +6422,7 @@
         <v>116</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rtr1-null</v>
       </c>
       <c r="F50" s="5" t="s">
@@ -6446,10 +6450,10 @@
         <v>72</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>59</v>
@@ -6491,17 +6495,17 @@
         <v>130</v>
       </c>
       <c r="AC50" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD50" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE50" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r1-n_Q_day8_tcn_N_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF50" s="1" t="str">
-        <f>_xlfn.CONCAT(F50, "_", P50, "_", T50, "_", AD50, "_", Y50, "_",  V50, "_", AA50, "_", I50, "_", O50)</f>
+        <f t="shared" si="5"/>
         <v>r1-n_Q_day8_tcn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG50" t="b">
@@ -6522,7 +6526,7 @@
         <v>56</v>
       </c>
       <c r="E51" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wild-type</v>
       </c>
       <c r="F51" s="5" t="s">
@@ -6550,10 +6554,10 @@
         <v>190</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>59</v>
@@ -6595,17 +6599,17 @@
         <v>130</v>
       </c>
       <c r="AC51" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD51" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE51" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WT_Q_day8_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF51" s="1" t="str">
-        <f>_xlfn.CONCAT(F51, "_", P51, "_", T51, "_", AD51, "_", Y51, "_",  V51, "_", AA51, "_", I51, "_", O51)</f>
+        <f t="shared" si="5"/>
         <v>WT_Q_day8_tcn_SS_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG51" t="b">
@@ -6626,7 +6630,7 @@
         <v>56</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wild-type</v>
       </c>
       <c r="F52" s="5" t="s">
@@ -6654,10 +6658,10 @@
         <v>190</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>59</v>
@@ -6699,17 +6703,17 @@
         <v>130</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD52" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE52" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WT_Q_day8_tcn_N_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF52" s="1" t="str">
-        <f>_xlfn.CONCAT(F52, "_", P52, "_", T52, "_", AD52, "_", Y52, "_",  V52, "_", AA52, "_", I52, "_", O52)</f>
+        <f t="shared" si="5"/>
         <v>WT_Q_day8_tcn_N_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG52" t="b">
@@ -6730,7 +6734,7 @@
         <v>56</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wild-type</v>
       </c>
       <c r="F53" s="5" t="s">
@@ -6749,19 +6753,19 @@
         <v>72</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>59</v>
@@ -6803,17 +6807,17 @@
         <v>130</v>
       </c>
       <c r="AC53" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD53" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE53" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WT_Q_day8_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF53" s="1" t="str">
-        <f>_xlfn.CONCAT(F53, "_", P53, "_", T53, "_", AD53, "_", Y53, "_",  V53, "_", AA53, "_", I53, "_", O53)</f>
+        <f t="shared" si="5"/>
         <v>WT_Q_day8_tcn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG53" t="b">
@@ -6834,7 +6838,7 @@
         <v>56</v>
       </c>
       <c r="E54" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>wild-type</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -6853,19 +6857,19 @@
         <v>72</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>59</v>
@@ -6907,17 +6911,17 @@
         <v>130</v>
       </c>
       <c r="AC54" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD54" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE54" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>WT_Q_day8_tcn_N_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF54" s="1" t="str">
-        <f>_xlfn.CONCAT(F54, "_", P54, "_", T54, "_", AD54, "_", Y54, "_",  V54, "_", AA54, "_", I54, "_", O54)</f>
+        <f t="shared" si="5"/>
         <v>WT_Q_day8_tcn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG54" t="b">
@@ -6925,103 +6929,103 @@
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C55" s="15">
         <v>7078</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="16" t="str">
-        <f t="shared" si="2"/>
+      <c r="E55" s="15" t="str">
+        <f t="shared" si="3"/>
         <v>rrp6-null</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="16" t="s">
+      <c r="G55" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="H55" s="16" t="s">
+      <c r="H55" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I55" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J55" s="16" t="s">
+      <c r="J55" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K55" s="16" t="s">
+      <c r="K55" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L55" s="17" t="s">
+      <c r="L55" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M55" s="16" t="s">
+      <c r="M55" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="N55" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="O55" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="P55" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q55" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="R55" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="S55" s="16" t="s">
+      <c r="N55" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="O55" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="P55" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q55" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="R55" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="S55" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T55" s="16" t="s">
+      <c r="T55" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="U55" s="16" t="s">
+      <c r="U55" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="V55" s="17" t="s">
+      <c r="V55" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="W55" s="16" t="s">
+      <c r="W55" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="X55" s="16" t="s">
+      <c r="X55" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y55" s="17" t="s">
+      <c r="Y55" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z55" s="16" t="s">
+      <c r="Z55" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA55" s="17" t="s">
+      <c r="AA55" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="AB55" s="16" t="s">
+      <c r="AB55" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="AC55" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD55" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE55" s="16" t="str">
+      <c r="AC55" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD55" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE55" s="15" t="str">
         <f>_xlfn.CONCAT(F55, "_", P55, "_", T55, "_", AD55, "_", Y55, "_",  V55, "_", AA55, "_", I55)</f>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
-      <c r="AF55" s="16" t="str">
-        <f>_xlfn.CONCAT(F55, "_", P55, "_", T55, "_", AD55, "_", Y55, "_",  V55, "_", AA55, "_", I55, "_", O55)</f>
+      <c r="AF55" s="15" t="str">
+        <f t="shared" si="5"/>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG55" s="12" t="b">
@@ -7029,105 +7033,105 @@
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B56" s="16" t="s">
+      <c r="A56" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C56" s="15">
         <v>7078</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="16" t="s">
+      <c r="G56" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="H56" s="16" t="s">
+      <c r="H56" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="I56" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J56" s="16" t="s">
+      <c r="J56" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K56" s="16" t="s">
+      <c r="K56" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L56" s="17" t="s">
+      <c r="L56" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M56" s="16" t="s">
+      <c r="M56" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="N56" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="O56" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="P56" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q56" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="R56" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="S56" s="16" t="s">
+      <c r="N56" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="O56" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="P56" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q56" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="R56" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="S56" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T56" s="16" t="s">
+      <c r="T56" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="U56" s="16" t="s">
+      <c r="U56" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="V56" s="18" t="s">
+      <c r="V56" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="W56" s="16" t="s">
+      <c r="W56" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="X56" s="16" t="s">
+      <c r="X56" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y56" s="17" t="s">
+      <c r="Y56" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z56" s="16" t="s">
+      <c r="Z56" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AA56" s="17" t="s">
+      <c r="AA56" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="AB56" s="16" t="s">
+      <c r="AB56" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="AC56" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD56" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE56" s="16" t="str">
+      <c r="AC56" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD56" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE56" s="15" t="str">
         <f>_xlfn.CONCAT(F56, "_", P56, "_", T56, "_", AD56, "_", Y56, "_",  V56, "_", AA56, "_", I56)</f>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
-      <c r="AF56" s="16" t="str">
-        <f>_xlfn.CONCAT(F56, "_", P56, "_", T56, "_", AD56, "_", Y56, "_",  V56, "_", AA56, "_", I56, "_", O56)</f>
+      <c r="AF56" s="15" t="str">
+        <f t="shared" si="5"/>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1_tech2</v>
       </c>
-      <c r="AG56" s="20" t="b">
+      <c r="AG56" s="19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7145,7 +7149,7 @@
         <v>106</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rrp6-null</v>
       </c>
       <c r="F57" s="5" t="s">
@@ -7173,10 +7177,10 @@
         <v>71</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P57" s="5" t="s">
         <v>59</v>
@@ -7218,17 +7222,17 @@
         <v>130</v>
       </c>
       <c r="AC57" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD57" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE57" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r6-n_Q_day8_tcn_N_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF57" s="1" t="str">
-        <f>_xlfn.CONCAT(F57, "_", P57, "_", T57, "_", AD57, "_", Y57, "_",  V57, "_", AA57, "_", I57, "_", O57)</f>
+        <f t="shared" si="5"/>
         <v>r6-n_Q_day8_tcn_N_aux-F_tc-F_rep1_tech1</v>
       </c>
       <c r="AG57" t="b">
@@ -7249,7 +7253,7 @@
         <v>106</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rrp6-null</v>
       </c>
       <c r="F58" s="5" t="s">
@@ -7277,10 +7281,10 @@
         <v>72</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>59</v>
@@ -7322,17 +7326,17 @@
         <v>130</v>
       </c>
       <c r="AC58" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD58" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE58" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF58" s="1" t="str">
-        <f>_xlfn.CONCAT(F58, "_", P58, "_", T58, "_", AD58, "_", Y58, "_",  V58, "_", AA58, "_", I58, "_", O58)</f>
+        <f t="shared" si="5"/>
         <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG58" t="b">
@@ -7353,7 +7357,7 @@
         <v>106</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>rrp6-null</v>
       </c>
       <c r="F59" s="5" t="s">
@@ -7381,10 +7385,10 @@
         <v>72</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>59</v>
@@ -7426,17 +7430,17 @@
         <v>130</v>
       </c>
       <c r="AC59" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD59" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE59" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r6-n_Q_day8_tcn_N_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF59" s="1" t="str">
-        <f>_xlfn.CONCAT(F59, "_", P59, "_", T59, "_", AD59, "_", Y59, "_",  V59, "_", AA59, "_", I59, "_", O59)</f>
+        <f t="shared" si="5"/>
         <v>r6-n_Q_day8_tcn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG59" t="b">
@@ -7445,10 +7449,10 @@
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="C60" s="1">
         <v>5781</v>
@@ -7483,11 +7487,11 @@
       <c r="M60" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N60" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>238</v>
+      <c r="N60" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O60" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>58</v>
@@ -7507,7 +7511,7 @@
       <c r="U60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V60" s="15" t="s">
+      <c r="V60" s="14" t="s">
         <v>97</v>
       </c>
       <c r="W60" s="1" t="s">
@@ -7529,29 +7533,29 @@
         <v>130</v>
       </c>
       <c r="AC60" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD60" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE60" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(F60, "_", P60, "_", T60, "_", AD60, "_", Y60, "_",  V60, "_", AA60, "_", I60)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF60" s="1" t="str">
         <f>_xlfn.CONCAT(F60, "_", P60, "_", T60, "_", AD60, "_", Y60, "_",  V60, "_", AA60, "_", I60, "_", O60)</f>
-        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech1</v>
-      </c>
-      <c r="AG60" s="19" t="b">
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
+      </c>
+      <c r="AG60" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="C61" s="1">
         <v>5782</v>
@@ -7586,11 +7590,11 @@
       <c r="M61" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N61" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>238</v>
+      <c r="N61" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O61" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="P61" s="5" t="s">
         <v>58</v>
@@ -7610,7 +7614,7 @@
       <c r="U61" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V61" s="15" t="s">
+      <c r="V61" s="14" t="s">
         <v>97</v>
       </c>
       <c r="W61" s="1" t="s">
@@ -7632,29 +7636,29 @@
         <v>130</v>
       </c>
       <c r="AC61" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD61" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE61" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(F61, "_", P61, "_", T61, "_", AD61, "_", Y61, "_",  V61, "_", AA61, "_", I61)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF61" s="1" t="str">
         <f>_xlfn.CONCAT(F61, "_", P61, "_", T61, "_", AD61, "_", Y61, "_",  V61, "_", AA61, "_", I61, "_", O61)</f>
-        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech1</v>
-      </c>
-      <c r="AG61" s="19" t="b">
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
+      </c>
+      <c r="AG61" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="C62" s="1">
         <v>7078</v>
@@ -7689,11 +7693,11 @@
       <c r="M62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N62" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>238</v>
+      <c r="N62" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O62" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>58</v>
@@ -7713,7 +7717,7 @@
       <c r="U62" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V62" s="15" t="s">
+      <c r="V62" s="14" t="s">
         <v>97</v>
       </c>
       <c r="W62" s="1" t="s">
@@ -7735,29 +7739,29 @@
         <v>130</v>
       </c>
       <c r="AC62" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD62" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE62" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(F62, "_", P62, "_", T62, "_", AD62, "_", Y62, "_",  V62, "_", AA62, "_", I62)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
       <c r="AF62" s="1" t="str">
         <f>_xlfn.CONCAT(F62, "_", P62, "_", T62, "_", AD62, "_", Y62, "_",  V62, "_", AA62, "_", I62, "_", O62)</f>
-        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech1</v>
-      </c>
-      <c r="AG62" s="19" t="b">
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
+      </c>
+      <c r="AG62" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="C63" s="1">
         <v>7079</v>
@@ -7792,11 +7796,11 @@
       <c r="M63" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N63" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>238</v>
+      <c r="N63" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O63" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>58</v>
@@ -7816,7 +7820,7 @@
       <c r="U63" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V63" s="15" t="s">
+      <c r="V63" s="14" t="s">
         <v>97</v>
       </c>
       <c r="W63" s="1" t="s">
@@ -7838,20 +7842,20 @@
         <v>130</v>
       </c>
       <c r="AC63" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AD63" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE63" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(F63, "_", P63, "_", T63, "_", AD63, "_", Y63, "_",  V63, "_", AA63, "_", I63)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF63" s="1" t="str">
         <f>_xlfn.CONCAT(F63, "_", P63, "_", T63, "_", AD63, "_", Y63, "_",  V63, "_", AA63, "_", I63, "_", O63)</f>
-        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech1</v>
-      </c>
-      <c r="AG63" s="19" t="b">
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
+      </c>
+      <c r="AG63" s="18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7867,107 +7871,1021 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082ED199-6BE6-DE4F-8415-858035711CE7}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A4589A-BEE9-F245-96E6-D3C48A34B761}">
+  <dimension ref="A1:AK38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="15">
+        <v>5781</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="AJ2" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="AK2" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7079</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AK7" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="15">
+        <v>7078</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="S12" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="T12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA12" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD12" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF12" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG12" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH12" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI12" s="15" t="str">
+        <f>_xlfn.CONCAT(J12, "_", T12, "_", X12, "_", AH12, "_", AC12, "_",  Z12, "_", AE12, "_", M12)</f>
+        <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1</v>
+      </c>
+      <c r="AJ12" s="15" t="str">
+        <f t="shared" ref="AJ12" si="0">_xlfn.CONCAT(J12, "_", T12, "_", X12, "_", AH12, "_", AC12, "_",  Z12, "_", AE12, "_", M12, "_", S12)</f>
+        <v>r6-n_Q_day8_tcn_SS_aux-F_tc-F_rep1_tech2</v>
+      </c>
+      <c r="AK12" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5781</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="S17" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z17" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI17" s="1" t="str">
+        <f>_xlfn.CONCAT(J17, "_", T17, "_", X17, "_", AH17, "_", AC17, "_",  Z17, "_", AE17, "_", M17)</f>
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
+      </c>
+      <c r="AJ17" s="1" t="str">
+        <f>_xlfn.CONCAT(J17, "_", T17, "_", X17, "_", AH17, "_", AC17, "_",  Z17, "_", AE17, "_", M17, "_", S17)</f>
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
+      </c>
+      <c r="AK17" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>238</v>
+      </c>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>239</v>
+      </c>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5782</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R22" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="S22" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI22" s="1" t="str">
+        <f>_xlfn.CONCAT(J22, "_", T22, "_", X22, "_", AH22, "_", AC22, "_",  Z22, "_", AE22, "_", M22)</f>
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AJ22" s="1" t="str">
+        <f>_xlfn.CONCAT(J22, "_", T22, "_", X22, "_", AH22, "_", AC22, "_",  Z22, "_", AE22, "_", M22, "_", S22)</f>
+        <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
+      </c>
+      <c r="AK22" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>243</v>
+      </c>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>244</v>
+      </c>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>246</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G27" s="1">
+        <v>7078</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R27" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="S27" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="T27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z27" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI27" s="1" t="str">
+        <f>_xlfn.CONCAT(J27, "_", T27, "_", X27, "_", AH27, "_", AC27, "_",  Z27, "_", AE27, "_", M27)</f>
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
+      </c>
+      <c r="AJ27" s="1" t="str">
+        <f>_xlfn.CONCAT(J27, "_", T27, "_", X27, "_", AH27, "_", AC27, "_",  Z27, "_", AE27, "_", M27, "_", S27)</f>
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
+      </c>
+      <c r="AK27" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>247</v>
+      </c>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>248</v>
+      </c>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>249</v>
+      </c>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>250</v>
+      </c>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G32" s="1">
+        <v>7079</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R32" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="S32" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z32" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG32" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" t="s">
-        <v>201</v>
+      <c r="AH32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI32" s="1" t="str">
+        <f>_xlfn.CONCAT(J32, "_", T32, "_", X32, "_", AH32, "_", AC32, "_",  Z32, "_", AE32, "_", M32)</f>
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
+      </c>
+      <c r="AJ32" s="1" t="str">
+        <f>_xlfn.CONCAT(J32, "_", T32, "_", X32, "_", AH32, "_", AC32, "_",  Z32, "_", AE32, "_", M32, "_", S32)</f>
+        <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
+      </c>
+      <c r="AK32" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated variables.xlsx to correct one minor name error
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE8AFE-540B-014E-9200-B433C90FDB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40920B12-CD88-1C44-A0B9-337EC55A3E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="500" windowWidth="47540" windowHeight="28300" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="262">
   <si>
     <t>5781_G1_IN</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>2023-0421: updated from tech1 to tech2</t>
+  </si>
+  <si>
+    <t>r6-n_DSp48_day4_tcn_SS_aux-F_tc-T_rep2_tech2</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -953,7 +956,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1286,7 +1288,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D52A0-EFB8-324D-84A5-D98AF0E44661}">
-  <dimension ref="A1:AG63"/>
+  <dimension ref="A1:AI63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -1327,7 +1329,7 @@
     <col min="33" max="33" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -1428,7 +1430,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1636,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1948,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2260,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>206</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2569,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>205</v>
       </c>
@@ -2663,14 +2665,15 @@
       <c r="AE13" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AF13" s="1" t="s">
-        <v>259</v>
+      <c r="AF13" s="20" t="s">
+        <v>261</v>
       </c>
       <c r="AG13" s="18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI13" s="1"/>
+    </row>
+    <row r="14" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2774,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -5981,11 +5984,11 @@
         <v>198</v>
       </c>
       <c r="AE45" s="1" t="str">
-        <f t="shared" ref="AE45:AE63" si="4">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45)</f>
+        <f t="shared" ref="AE45:AE59" si="4">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45)</f>
         <v>WT_Q_day7_tcn_N_aux-F_tc-F_rep2</v>
       </c>
       <c r="AF45" s="1" t="str">
-        <f t="shared" ref="AF45:AF63" si="5">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45, "_", O45)</f>
+        <f t="shared" ref="AF45:AF59" si="5">_xlfn.CONCAT(F45, "_", P45, "_", T45, "_", AD45, "_", Y45, "_",  V45, "_", AA45, "_", I45, "_", O45)</f>
         <v>WT_Q_day7_tcn_N_aux-F_tc-F_rep2_tech1</v>
       </c>
       <c r="AG45" t="b">
@@ -7542,7 +7545,7 @@
         <f>_xlfn.CONCAT(F60, "_", P60, "_", T60, "_", AD60, "_", Y60, "_",  V60, "_", AA60, "_", I60)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
-      <c r="AF60" s="1" t="str">
+      <c r="AF60" s="20" t="str">
         <f>_xlfn.CONCAT(F60, "_", P60, "_", T60, "_", AD60, "_", Y60, "_",  V60, "_", AA60, "_", I60, "_", O60)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
       </c>
@@ -7645,7 +7648,7 @@
         <f>_xlfn.CONCAT(F61, "_", P61, "_", T61, "_", AD61, "_", Y61, "_",  V61, "_", AA61, "_", I61)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
-      <c r="AF61" s="1" t="str">
+      <c r="AF61" s="20" t="str">
         <f>_xlfn.CONCAT(F61, "_", P61, "_", T61, "_", AD61, "_", Y61, "_",  V61, "_", AA61, "_", I61, "_", O61)</f>
         <v>WT_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
       </c>
@@ -7748,7 +7751,7 @@
         <f>_xlfn.CONCAT(F62, "_", P62, "_", T62, "_", AD62, "_", Y62, "_",  V62, "_", AA62, "_", I62)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1</v>
       </c>
-      <c r="AF62" s="1" t="str">
+      <c r="AF62" s="20" t="str">
         <f>_xlfn.CONCAT(F62, "_", P62, "_", T62, "_", AD62, "_", Y62, "_",  V62, "_", AA62, "_", I62, "_", O62)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep1_tech2</v>
       </c>
@@ -7851,7 +7854,7 @@
         <f>_xlfn.CONCAT(F63, "_", P63, "_", T63, "_", AD63, "_", Y63, "_",  V63, "_", AA63, "_", I63)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2</v>
       </c>
-      <c r="AF63" s="1" t="str">
+      <c r="AF63" s="20" t="str">
         <f>_xlfn.CONCAT(F63, "_", P63, "_", T63, "_", AD63, "_", Y63, "_",  V63, "_", AA63, "_", I63, "_", O63)</f>
         <v>r6-n_G1_day1_tcn_SS_aux-F_tc-F_rep2_tech2</v>
       </c>
@@ -8465,29 +8468,21 @@
       <c r="A18" t="s">
         <v>237</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>238</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>239</v>
       </c>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>240</v>
       </c>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -8599,29 +8594,21 @@
       <c r="A23" t="s">
         <v>242</v>
       </c>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>243</v>
       </c>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>244</v>
       </c>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>245</v>
       </c>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -8733,29 +8720,21 @@
       <c r="A28" t="s">
         <v>247</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>248</v>
       </c>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>249</v>
       </c>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>250</v>
       </c>
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Moving forward with the rlog/PCA work; in referencing old code, cleaned things up a bit; also, finally corrected replicate names per Alison's notes (see e-mail thread with title 'Quick guide to know what 4tU-seq filenames represent what'
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/variables.xlsx
+++ b/results/2023-0215/notebook/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40920B12-CD88-1C44-A0B9-337EC55A3E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F5010C-2AEB-6340-9931-7958BAF4DAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="28300" xr2:uid="{8624B68D-0A8F-7B47-BB3D-1ED5459CAF57}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -1290,7 +1290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D52A0-EFB8-324D-84A5-D98AF0E44661}">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:D36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4858,16 +4860,16 @@
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>7718</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -4961,16 +4963,16 @@
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="3">
         <v>7718</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E36" s="3" t="s">

</xml_diff>